<commit_message>
Fixed ThinningRule, metrics, Shepparton
</commit_message>
<xml_diff>
--- a/Tests/Validation/Eucalyptus/Observed.xlsx
+++ b/Tests/Validation/Eucalyptus/Observed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Tests\Validation\Eucalyptus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMx Temporary Work Area\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D379089-56E8-40D9-8FC0-F6E637502F9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2515ED-874C-4991-B9EE-FF87951551F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -966,7 +966,7 @@
     <numFmt numFmtId="165" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
-    <numFmt numFmtId="169" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -1131,7 +1131,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1157,15 +1157,6 @@
     <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1180,6 +1171,15 @@
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -17563,18 +17563,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:12" ht="29.25" thickBot="1">
       <c r="B3" s="9" t="s">
@@ -17597,7 +17597,7 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="35" t="s">
         <v>83</v>
       </c>
       <c r="B4" s="11">
@@ -17620,7 +17620,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="30"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="12">
         <v>2</v>
       </c>
@@ -17644,7 +17644,7 @@
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="35" t="s">
         <v>84</v>
       </c>
       <c r="B6" s="13">
@@ -17661,7 +17661,7 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="30"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="13">
         <v>2</v>
       </c>
@@ -17676,7 +17676,7 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="30"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="13">
         <v>3</v>
       </c>
@@ -17691,7 +17691,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="37" t="s">
         <v>166</v>
       </c>
       <c r="B9" s="13">
@@ -17711,7 +17711,7 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="30"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="13">
         <v>2</v>
       </c>
@@ -17729,7 +17729,7 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="35" t="s">
         <v>85</v>
       </c>
       <c r="B11" s="13">
@@ -17746,7 +17746,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="30"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="13">
         <v>2</v>
       </c>
@@ -17761,7 +17761,7 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="30"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="13">
         <v>3</v>
       </c>
@@ -17776,7 +17776,7 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="35" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="13">
@@ -17793,7 +17793,7 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="30"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="13">
         <v>2</v>
       </c>
@@ -17808,7 +17808,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="30"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="13">
         <v>3</v>
       </c>
@@ -17823,7 +17823,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="35" t="s">
         <v>87</v>
       </c>
       <c r="B17" s="13">
@@ -17840,7 +17840,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="30"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="13">
         <v>2</v>
       </c>
@@ -17855,7 +17855,7 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="30"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="13">
         <v>3</v>
       </c>
@@ -17870,7 +17870,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="35" t="s">
         <v>88</v>
       </c>
       <c r="B20" s="13">
@@ -17887,7 +17887,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15">
-      <c r="A21" s="30"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="13">
         <v>2</v>
       </c>
@@ -17902,7 +17902,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15">
-      <c r="A22" s="30"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="13">
         <v>3</v>
       </c>
@@ -17917,7 +17917,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="35" t="s">
         <v>89</v>
       </c>
       <c r="B23" s="13">
@@ -17943,7 +17943,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="30"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="13">
         <v>2</v>
       </c>
@@ -17967,7 +17967,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="30"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="13">
         <v>3</v>
       </c>
@@ -17991,7 +17991,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="35" t="s">
         <v>90</v>
       </c>
       <c r="B26" s="13">
@@ -18017,7 +18017,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="30"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="13">
         <v>2</v>
       </c>
@@ -18032,7 +18032,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="30"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="13">
         <v>3</v>
       </c>
@@ -18047,7 +18047,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="35" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="13">
@@ -18064,7 +18064,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="30"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="13">
         <v>2</v>
       </c>
@@ -18079,7 +18079,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="30"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="13">
         <v>3</v>
       </c>
@@ -18094,7 +18094,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B32" s="13">
@@ -18111,7 +18111,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="30"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="13">
         <v>2</v>
       </c>
@@ -18126,7 +18126,7 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="30"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="13">
         <v>3</v>
       </c>
@@ -18165,10 +18165,10 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:BS2650"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="510" topLeftCell="A2" activePane="bottomLeft"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <pane ySplit="510" topLeftCell="A1250" activePane="bottomLeft"/>
+      <selection activeCell="AJ1" sqref="AJ1"/>
+      <selection pane="bottomLeft" activeCell="AJ1227" sqref="AJ1227:AJ1278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -24365,11 +24365,11 @@
         <v>6.2</v>
       </c>
       <c r="D173" s="28"/>
-      <c r="F173" s="33"/>
-      <c r="M173" s="34"/>
-      <c r="N173" s="34"/>
-      <c r="O173" s="34"/>
-      <c r="P173" s="34"/>
+      <c r="F173" s="30"/>
+      <c r="M173" s="31"/>
+      <c r="N173" s="31"/>
+      <c r="O173" s="31"/>
+      <c r="P173" s="31"/>
       <c r="W173" s="21">
         <v>8.27</v>
       </c>
@@ -24385,10 +24385,10 @@
         <v>7.05</v>
       </c>
       <c r="D174" s="28"/>
-      <c r="M174" s="34"/>
-      <c r="N174" s="34"/>
-      <c r="O174" s="34"/>
-      <c r="P174" s="34"/>
+      <c r="M174" s="31"/>
+      <c r="N174" s="31"/>
+      <c r="O174" s="31"/>
+      <c r="P174" s="31"/>
       <c r="W174" s="21">
         <v>7.17</v>
       </c>
@@ -24404,8 +24404,8 @@
         <v>7.44</v>
       </c>
       <c r="D175" s="28"/>
-      <c r="O175" s="34"/>
-      <c r="P175" s="34"/>
+      <c r="O175" s="31"/>
+      <c r="P175" s="31"/>
       <c r="W175" s="21">
         <v>7.02</v>
       </c>
@@ -24421,8 +24421,8 @@
         <v>7.87</v>
       </c>
       <c r="D176" s="28"/>
-      <c r="O176" s="34"/>
-      <c r="P176" s="34"/>
+      <c r="O176" s="31"/>
+      <c r="P176" s="31"/>
       <c r="W176" s="21">
         <v>7.19</v>
       </c>
@@ -24438,9 +24438,9 @@
         <v>5.58</v>
       </c>
       <c r="D177" s="28"/>
-      <c r="N177" s="34"/>
-      <c r="O177" s="34"/>
-      <c r="P177" s="34"/>
+      <c r="N177" s="31"/>
+      <c r="O177" s="31"/>
+      <c r="P177" s="31"/>
       <c r="W177" s="21">
         <v>8.31</v>
       </c>
@@ -24456,9 +24456,9 @@
         <v>6.2</v>
       </c>
       <c r="D178" s="28"/>
-      <c r="N178" s="34"/>
-      <c r="O178" s="34"/>
-      <c r="P178" s="34"/>
+      <c r="N178" s="31"/>
+      <c r="O178" s="31"/>
+      <c r="P178" s="31"/>
       <c r="W178" s="21">
         <v>8.41</v>
       </c>
@@ -24474,8 +24474,8 @@
         <v>7.05</v>
       </c>
       <c r="D179" s="28"/>
-      <c r="O179" s="34"/>
-      <c r="P179" s="34"/>
+      <c r="O179" s="31"/>
+      <c r="P179" s="31"/>
       <c r="W179" s="21">
         <v>7.2</v>
       </c>
@@ -24491,8 +24491,8 @@
         <v>7.44</v>
       </c>
       <c r="D180" s="28"/>
-      <c r="O180" s="34"/>
-      <c r="P180" s="34"/>
+      <c r="O180" s="31"/>
+      <c r="P180" s="31"/>
       <c r="W180" s="21">
         <v>7.2</v>
       </c>
@@ -24508,8 +24508,8 @@
         <v>7.87</v>
       </c>
       <c r="D181" s="28"/>
-      <c r="O181" s="34"/>
-      <c r="P181" s="34"/>
+      <c r="O181" s="31"/>
+      <c r="P181" s="31"/>
       <c r="W181" s="21">
         <v>7.34</v>
       </c>
@@ -24525,8 +24525,8 @@
         <v>0.24914442162902123</v>
       </c>
       <c r="D182" s="28"/>
-      <c r="O182" s="34"/>
-      <c r="P182" s="34"/>
+      <c r="O182" s="31"/>
+      <c r="P182" s="31"/>
       <c r="BH182" s="21">
         <v>3.3352009052827341</v>
       </c>
@@ -24542,9 +24542,9 @@
         <v>0.3613963039014374</v>
       </c>
       <c r="D183" s="28"/>
-      <c r="N183" s="34"/>
-      <c r="O183" s="34"/>
-      <c r="P183" s="34"/>
+      <c r="N183" s="31"/>
+      <c r="O183" s="31"/>
+      <c r="P183" s="31"/>
       <c r="BH183" s="21">
         <v>5.3378061780489672</v>
       </c>
@@ -24560,9 +24560,9 @@
         <v>0.47091033538672145</v>
       </c>
       <c r="D184" s="28"/>
-      <c r="N184" s="34"/>
-      <c r="O184" s="34"/>
-      <c r="P184" s="34"/>
+      <c r="N184" s="31"/>
+      <c r="O184" s="31"/>
+      <c r="P184" s="31"/>
       <c r="BH184" s="21">
         <v>8.0304225893924048</v>
       </c>
@@ -24578,8 +24578,8 @@
         <v>0.68446269678302529</v>
       </c>
       <c r="D185" s="28"/>
-      <c r="O185" s="34"/>
-      <c r="P185" s="34"/>
+      <c r="O185" s="31"/>
+      <c r="P185" s="31"/>
       <c r="BH185" s="21">
         <v>4.5584479475526019</v>
       </c>
@@ -24595,8 +24595,8 @@
         <v>0.84052019164955505</v>
       </c>
       <c r="D186" s="28"/>
-      <c r="O186" s="34"/>
-      <c r="P186" s="34"/>
+      <c r="O186" s="31"/>
+      <c r="P186" s="31"/>
       <c r="BH186" s="21">
         <v>3.1607358328057575</v>
       </c>
@@ -24612,8 +24612,8 @@
         <v>1.6427104722792607</v>
       </c>
       <c r="D187" s="28"/>
-      <c r="O187" s="34"/>
-      <c r="P187" s="34"/>
+      <c r="O187" s="31"/>
+      <c r="P187" s="31"/>
       <c r="BH187" s="21">
         <v>1.5050467837428154E-2</v>
       </c>
@@ -24629,8 +24629,8 @@
         <v>2.0314852840520192</v>
       </c>
       <c r="D188" s="28"/>
-      <c r="O188" s="34"/>
-      <c r="P188" s="34"/>
+      <c r="O188" s="31"/>
+      <c r="P188" s="31"/>
       <c r="BH188" s="21">
         <v>1.276506997960839E-2</v>
       </c>
@@ -24646,8 +24646,8 @@
         <v>2.1108829568788501</v>
       </c>
       <c r="D189" s="28"/>
-      <c r="O189" s="34"/>
-      <c r="P189" s="34"/>
+      <c r="O189" s="31"/>
+      <c r="P189" s="31"/>
       <c r="BH189" s="21">
         <v>2.20123697901893E-2</v>
       </c>
@@ -24663,10 +24663,10 @@
         <v>2.2450376454483232</v>
       </c>
       <c r="D190" s="28"/>
-      <c r="M190" s="34"/>
-      <c r="N190" s="34"/>
-      <c r="O190" s="34"/>
-      <c r="P190" s="34"/>
+      <c r="M190" s="31"/>
+      <c r="N190" s="31"/>
+      <c r="O190" s="31"/>
+      <c r="P190" s="31"/>
       <c r="BH190" s="21">
         <v>2.8262423511851147E-2</v>
       </c>
@@ -24682,10 +24682,10 @@
         <v>2.3764544832306638</v>
       </c>
       <c r="D191" s="28"/>
-      <c r="M191" s="34"/>
-      <c r="N191" s="34"/>
-      <c r="O191" s="34"/>
-      <c r="P191" s="34"/>
+      <c r="M191" s="31"/>
+      <c r="N191" s="31"/>
+      <c r="O191" s="31"/>
+      <c r="P191" s="31"/>
       <c r="BH191" s="21">
         <v>1.7682570570030833E-2</v>
       </c>
@@ -24701,8 +24701,8 @@
         <v>2.6064339493497606</v>
       </c>
       <c r="D192" s="28"/>
-      <c r="O192" s="34"/>
-      <c r="P192" s="34"/>
+      <c r="O192" s="31"/>
+      <c r="P192" s="31"/>
       <c r="BH192" s="21">
         <v>1.7421730850087128E-3</v>
       </c>
@@ -24718,8 +24718,8 @@
         <v>2.9322381930184807</v>
       </c>
       <c r="D193" s="28"/>
-      <c r="O193" s="34"/>
-      <c r="P193" s="34"/>
+      <c r="O193" s="31"/>
+      <c r="P193" s="31"/>
       <c r="BH193" s="21">
         <v>3.1491859124216435E-3</v>
       </c>
@@ -24735,10 +24735,10 @@
         <v>3.1759069130732374</v>
       </c>
       <c r="D194" s="28"/>
-      <c r="M194" s="35"/>
-      <c r="N194" s="35"/>
-      <c r="O194" s="34"/>
-      <c r="P194" s="34"/>
+      <c r="M194" s="32"/>
+      <c r="N194" s="32"/>
+      <c r="O194" s="31"/>
+      <c r="P194" s="31"/>
       <c r="BH194" s="21">
         <v>8.2719385594224161E-4</v>
       </c>
@@ -24754,10 +24754,10 @@
         <v>3.5208761122518824</v>
       </c>
       <c r="D195" s="28"/>
-      <c r="M195" s="35"/>
-      <c r="N195" s="35"/>
-      <c r="O195" s="34"/>
-      <c r="P195" s="34"/>
+      <c r="M195" s="32"/>
+      <c r="N195" s="32"/>
+      <c r="O195" s="31"/>
+      <c r="P195" s="31"/>
       <c r="BH195" s="21">
         <v>7.8821646033169299E-3</v>
       </c>
@@ -24773,10 +24773,10 @@
         <v>3.7563312799452429</v>
       </c>
       <c r="D196" s="28"/>
-      <c r="M196" s="35"/>
-      <c r="N196" s="35"/>
-      <c r="O196" s="34"/>
-      <c r="P196" s="34"/>
+      <c r="M196" s="32"/>
+      <c r="N196" s="32"/>
+      <c r="O196" s="31"/>
+      <c r="P196" s="31"/>
       <c r="BH196" s="21">
         <v>1.5767542127177923E-3</v>
       </c>
@@ -24792,10 +24792,10 @@
         <v>4.0958247775496233</v>
       </c>
       <c r="D197" s="28"/>
-      <c r="M197" s="35"/>
-      <c r="N197" s="34"/>
-      <c r="O197" s="34"/>
-      <c r="P197" s="34"/>
+      <c r="M197" s="32"/>
+      <c r="N197" s="31"/>
+      <c r="O197" s="31"/>
+      <c r="P197" s="31"/>
       <c r="BH197" s="21">
         <v>1.1673992232268322E-3</v>
       </c>
@@ -24811,10 +24811,10 @@
         <v>0.24914442162902123</v>
       </c>
       <c r="D198" s="28"/>
-      <c r="M198" s="35"/>
-      <c r="N198" s="34"/>
-      <c r="O198" s="34"/>
-      <c r="P198" s="34"/>
+      <c r="M198" s="32"/>
+      <c r="N198" s="31"/>
+      <c r="O198" s="31"/>
+      <c r="P198" s="31"/>
       <c r="BH198" s="21">
         <v>3.4278499267179461</v>
       </c>
@@ -24830,8 +24830,8 @@
         <v>0.3613963039014374</v>
       </c>
       <c r="D199" s="28"/>
-      <c r="O199" s="34"/>
-      <c r="P199" s="34"/>
+      <c r="O199" s="31"/>
+      <c r="P199" s="31"/>
       <c r="BH199" s="21">
         <v>5.2203160861809872</v>
       </c>
@@ -24847,8 +24847,8 @@
         <v>0.47091033538672145</v>
       </c>
       <c r="D200" s="28"/>
-      <c r="O200" s="34"/>
-      <c r="P200" s="34"/>
+      <c r="O200" s="31"/>
+      <c r="P200" s="31"/>
       <c r="BH200" s="21">
         <v>5.1297015705723767</v>
       </c>
@@ -24864,10 +24864,10 @@
         <v>0.84052019164955505</v>
       </c>
       <c r="D201" s="28"/>
-      <c r="M201" s="35"/>
-      <c r="N201" s="35"/>
-      <c r="O201" s="34"/>
-      <c r="P201" s="34"/>
+      <c r="M201" s="32"/>
+      <c r="N201" s="32"/>
+      <c r="O201" s="31"/>
+      <c r="P201" s="31"/>
       <c r="BH201" s="21">
         <v>1.4970510148410185</v>
       </c>
@@ -24883,10 +24883,10 @@
         <v>2.0314852840520192</v>
       </c>
       <c r="D202" s="28"/>
-      <c r="M202" s="35"/>
-      <c r="N202" s="35"/>
-      <c r="O202" s="34"/>
-      <c r="P202" s="34"/>
+      <c r="M202" s="32"/>
+      <c r="N202" s="32"/>
+      <c r="O202" s="31"/>
+      <c r="P202" s="31"/>
       <c r="BH202" s="21">
         <v>8.2476476678703843E-3</v>
       </c>
@@ -24902,11 +24902,11 @@
         <v>2.1108829568788501</v>
       </c>
       <c r="D203" s="28"/>
-      <c r="F203" s="33"/>
-      <c r="M203" s="34"/>
-      <c r="N203" s="34"/>
-      <c r="O203" s="34"/>
-      <c r="P203" s="34"/>
+      <c r="F203" s="30"/>
+      <c r="M203" s="31"/>
+      <c r="N203" s="31"/>
+      <c r="O203" s="31"/>
+      <c r="P203" s="31"/>
       <c r="BH203" s="21">
         <v>0.10537842420849793</v>
       </c>
@@ -24922,10 +24922,10 @@
         <v>2.2450376454483232</v>
       </c>
       <c r="D204" s="28"/>
-      <c r="M204" s="34"/>
-      <c r="N204" s="34"/>
-      <c r="O204" s="34"/>
-      <c r="P204" s="34"/>
+      <c r="M204" s="31"/>
+      <c r="N204" s="31"/>
+      <c r="O204" s="31"/>
+      <c r="P204" s="31"/>
       <c r="BH204" s="21">
         <v>0.18206283454524325</v>
       </c>
@@ -24941,8 +24941,8 @@
         <v>2.3764544832306638</v>
       </c>
       <c r="D205" s="28"/>
-      <c r="O205" s="34"/>
-      <c r="P205" s="34"/>
+      <c r="O205" s="31"/>
+      <c r="P205" s="31"/>
       <c r="BH205" s="21">
         <v>9.4621864181857699E-3</v>
       </c>
@@ -24958,9 +24958,9 @@
         <v>2.6064339493497606</v>
       </c>
       <c r="D206" s="28"/>
-      <c r="N206" s="34"/>
-      <c r="O206" s="34"/>
-      <c r="P206" s="34"/>
+      <c r="N206" s="31"/>
+      <c r="O206" s="31"/>
+      <c r="P206" s="31"/>
       <c r="BH206" s="21">
         <v>8.497981865892533E-4</v>
       </c>
@@ -24976,9 +24976,9 @@
         <v>2.9322381930184807</v>
       </c>
       <c r="D207" s="28"/>
-      <c r="N207" s="34"/>
-      <c r="O207" s="34"/>
-      <c r="P207" s="34"/>
+      <c r="N207" s="31"/>
+      <c r="O207" s="31"/>
+      <c r="P207" s="31"/>
       <c r="BH207" s="21">
         <v>1.8165397263731756E-3</v>
       </c>
@@ -24994,8 +24994,8 @@
         <v>3.1759069130732374</v>
       </c>
       <c r="D208" s="28"/>
-      <c r="O208" s="34"/>
-      <c r="P208" s="34"/>
+      <c r="O208" s="31"/>
+      <c r="P208" s="31"/>
       <c r="BH208" s="21">
         <v>8.3449588603376338E-4</v>
       </c>
@@ -25011,9 +25011,9 @@
         <v>3.5208761122518824</v>
       </c>
       <c r="D209" s="28"/>
-      <c r="M209" s="34"/>
-      <c r="O209" s="34"/>
-      <c r="P209" s="34"/>
+      <c r="M209" s="31"/>
+      <c r="O209" s="31"/>
+      <c r="P209" s="31"/>
       <c r="BH209" s="21">
         <v>5.6687186159300193E-3</v>
       </c>
@@ -25029,9 +25029,9 @@
         <v>3.7563312799452429</v>
       </c>
       <c r="D210" s="28"/>
-      <c r="M210" s="34"/>
-      <c r="O210" s="34"/>
-      <c r="P210" s="34"/>
+      <c r="M210" s="31"/>
+      <c r="O210" s="31"/>
+      <c r="P210" s="31"/>
       <c r="BH210" s="21">
         <v>8.3011889634349782E-4</v>
       </c>
@@ -25047,8 +25047,8 @@
         <v>4.0958247775496233</v>
       </c>
       <c r="D211" s="28"/>
-      <c r="O211" s="34"/>
-      <c r="P211" s="34"/>
+      <c r="O211" s="31"/>
+      <c r="P211" s="31"/>
       <c r="BH211" s="21">
         <v>8.1641918193268374E-4</v>
       </c>
@@ -25064,8 +25064,8 @@
         <v>0.24914442162902123</v>
       </c>
       <c r="D212" s="28"/>
-      <c r="O212" s="34"/>
-      <c r="P212" s="34"/>
+      <c r="O212" s="31"/>
+      <c r="P212" s="31"/>
       <c r="BH212" s="21">
         <v>2.6938648278388793</v>
       </c>
@@ -25081,9 +25081,9 @@
         <v>0.3613963039014374</v>
       </c>
       <c r="D213" s="28"/>
-      <c r="N213" s="34"/>
-      <c r="O213" s="34"/>
-      <c r="P213" s="34"/>
+      <c r="N213" s="31"/>
+      <c r="O213" s="31"/>
+      <c r="P213" s="31"/>
       <c r="BH213" s="21">
         <v>6.452122435962548</v>
       </c>
@@ -25099,9 +25099,9 @@
         <v>0.47091033538672145</v>
       </c>
       <c r="D214" s="28"/>
-      <c r="N214" s="34"/>
-      <c r="O214" s="34"/>
-      <c r="P214" s="34"/>
+      <c r="N214" s="31"/>
+      <c r="O214" s="31"/>
+      <c r="P214" s="31"/>
       <c r="BH214" s="21">
         <v>5.1018172749436133</v>
       </c>
@@ -25117,8 +25117,8 @@
         <v>0.84052019164955505</v>
       </c>
       <c r="D215" s="28"/>
-      <c r="O215" s="34"/>
-      <c r="P215" s="34"/>
+      <c r="O215" s="31"/>
+      <c r="P215" s="31"/>
       <c r="BH215" s="21">
         <v>1.7424952383830152</v>
       </c>
@@ -25134,8 +25134,8 @@
         <v>2.0314852840520192</v>
       </c>
       <c r="D216" s="28"/>
-      <c r="O216" s="34"/>
-      <c r="P216" s="34"/>
+      <c r="O216" s="31"/>
+      <c r="P216" s="31"/>
       <c r="BH216" s="21">
         <v>3.739454041136236E-3</v>
       </c>
@@ -25151,8 +25151,8 @@
         <v>2.1108829568788501</v>
       </c>
       <c r="D217" s="28"/>
-      <c r="O217" s="34"/>
-      <c r="P217" s="34"/>
+      <c r="O217" s="31"/>
+      <c r="P217" s="31"/>
       <c r="BH217" s="21">
         <v>9.7777313376750483E-2</v>
       </c>
@@ -25168,8 +25168,8 @@
         <v>2.2450376454483232</v>
       </c>
       <c r="D218" s="28"/>
-      <c r="O218" s="34"/>
-      <c r="P218" s="34"/>
+      <c r="O218" s="31"/>
+      <c r="P218" s="31"/>
       <c r="BH218" s="21">
         <v>0.20288923283812227</v>
       </c>
@@ -25185,10 +25185,10 @@
         <v>2.3764544832306638</v>
       </c>
       <c r="D219" s="28"/>
-      <c r="M219" s="34"/>
-      <c r="N219" s="34"/>
-      <c r="O219" s="34"/>
-      <c r="P219" s="34"/>
+      <c r="M219" s="31"/>
+      <c r="N219" s="31"/>
+      <c r="O219" s="31"/>
+      <c r="P219" s="31"/>
       <c r="BH219" s="21">
         <v>2.9056499987877918E-2</v>
       </c>
@@ -25204,10 +25204,10 @@
         <v>2.6064339493497606</v>
       </c>
       <c r="D220" s="28"/>
-      <c r="M220" s="34"/>
-      <c r="N220" s="34"/>
-      <c r="O220" s="34"/>
-      <c r="P220" s="34"/>
+      <c r="M220" s="31"/>
+      <c r="N220" s="31"/>
+      <c r="O220" s="31"/>
+      <c r="P220" s="31"/>
       <c r="BH220" s="21">
         <v>1.5482489708569375E-3</v>
       </c>
@@ -25223,8 +25223,8 @@
         <v>2.9322381930184807</v>
       </c>
       <c r="D221" s="28"/>
-      <c r="O221" s="34"/>
-      <c r="P221" s="34"/>
+      <c r="O221" s="31"/>
+      <c r="P221" s="31"/>
       <c r="BH221" s="21">
         <v>5.7773156985987386E-3</v>
       </c>
@@ -25240,8 +25240,8 @@
         <v>3.1759069130732374</v>
       </c>
       <c r="D222" s="28"/>
-      <c r="O222" s="34"/>
-      <c r="P222" s="34"/>
+      <c r="O222" s="31"/>
+      <c r="P222" s="31"/>
       <c r="BH222" s="21">
         <v>8.2153032670159742E-4</v>
       </c>
@@ -25257,10 +25257,10 @@
         <v>3.5208761122518824</v>
       </c>
       <c r="D223" s="28"/>
-      <c r="M223" s="35"/>
-      <c r="N223" s="35"/>
-      <c r="O223" s="34"/>
-      <c r="P223" s="34"/>
+      <c r="M223" s="32"/>
+      <c r="N223" s="32"/>
+      <c r="O223" s="31"/>
+      <c r="P223" s="31"/>
       <c r="BH223" s="21">
         <v>6.0908779903161292E-3</v>
       </c>
@@ -25276,10 +25276,10 @@
         <v>3.7563312799452429</v>
       </c>
       <c r="D224" s="28"/>
-      <c r="M224" s="35"/>
-      <c r="N224" s="35"/>
-      <c r="O224" s="34"/>
-      <c r="P224" s="34"/>
+      <c r="M224" s="32"/>
+      <c r="N224" s="32"/>
+      <c r="O224" s="31"/>
+      <c r="P224" s="31"/>
       <c r="BH224" s="21">
         <v>8.1727177398017818E-4</v>
       </c>
@@ -25295,10 +25295,10 @@
         <v>4.0958247775496233</v>
       </c>
       <c r="D225" s="28"/>
-      <c r="M225" s="35"/>
-      <c r="N225" s="35"/>
-      <c r="O225" s="34"/>
-      <c r="P225" s="34"/>
+      <c r="M225" s="32"/>
+      <c r="N225" s="32"/>
+      <c r="O225" s="31"/>
+      <c r="P225" s="31"/>
       <c r="BH225" s="21">
         <v>1.1679178605533773E-3</v>
       </c>
@@ -25314,10 +25314,10 @@
         <v>0.24914442162902123</v>
       </c>
       <c r="D226" s="28"/>
-      <c r="M226" s="35"/>
-      <c r="N226" s="35"/>
-      <c r="O226" s="34"/>
-      <c r="P226" s="34"/>
+      <c r="M226" s="32"/>
+      <c r="N226" s="32"/>
+      <c r="O226" s="31"/>
+      <c r="P226" s="31"/>
       <c r="BH226" s="21">
         <v>1.5960658302495594</v>
       </c>
@@ -25333,10 +25333,10 @@
         <v>0.3613963039014374</v>
       </c>
       <c r="D227" s="28"/>
-      <c r="M227" s="35"/>
-      <c r="N227" s="34"/>
-      <c r="O227" s="34"/>
-      <c r="P227" s="34"/>
+      <c r="M227" s="32"/>
+      <c r="N227" s="31"/>
+      <c r="O227" s="31"/>
+      <c r="P227" s="31"/>
       <c r="BH227" s="21">
         <v>2.0466595203545253</v>
       </c>
@@ -25352,10 +25352,10 @@
         <v>0.47091033538672145</v>
       </c>
       <c r="D228" s="28"/>
-      <c r="M228" s="35"/>
-      <c r="N228" s="34"/>
-      <c r="O228" s="34"/>
-      <c r="P228" s="34"/>
+      <c r="M228" s="32"/>
+      <c r="N228" s="31"/>
+      <c r="O228" s="31"/>
+      <c r="P228" s="31"/>
       <c r="BH228" s="21">
         <v>4.5401834369107927</v>
       </c>
@@ -25371,8 +25371,8 @@
         <v>0.84052019164955505</v>
       </c>
       <c r="D229" s="28"/>
-      <c r="O229" s="36"/>
-      <c r="P229" s="36"/>
+      <c r="O229" s="33"/>
+      <c r="P229" s="33"/>
       <c r="BH229" s="21">
         <v>2.5681216967828662</v>
       </c>
@@ -25388,8 +25388,8 @@
         <v>2.0314852840520192</v>
       </c>
       <c r="D230" s="28"/>
-      <c r="O230" s="36"/>
-      <c r="P230" s="36"/>
+      <c r="O230" s="33"/>
+      <c r="P230" s="33"/>
       <c r="BH230" s="21">
         <v>2.4229664463747817E-3</v>
       </c>
@@ -25405,8 +25405,8 @@
         <v>2.1108829568788501</v>
       </c>
       <c r="D231" s="28"/>
-      <c r="O231" s="36"/>
-      <c r="P231" s="36"/>
+      <c r="O231" s="33"/>
+      <c r="P231" s="33"/>
       <c r="BH231" s="21">
         <v>0.20927478286751297</v>
       </c>
@@ -25422,8 +25422,8 @@
         <v>2.2450376454483232</v>
       </c>
       <c r="D232" s="28"/>
-      <c r="O232" s="36"/>
-      <c r="P232" s="36"/>
+      <c r="O232" s="33"/>
+      <c r="P232" s="33"/>
       <c r="BH232" s="21">
         <v>1.3752510968520772</v>
       </c>
@@ -25439,8 +25439,8 @@
         <v>2.3764544832306638</v>
       </c>
       <c r="D233" s="28"/>
-      <c r="O233" s="36"/>
-      <c r="P233" s="36"/>
+      <c r="O233" s="33"/>
+      <c r="P233" s="33"/>
       <c r="BH233" s="21">
         <v>0.78560945201600973</v>
       </c>
@@ -25456,8 +25456,8 @@
         <v>2.6064339493497606</v>
       </c>
       <c r="D234" s="28"/>
-      <c r="O234" s="36"/>
-      <c r="P234" s="36"/>
+      <c r="O234" s="33"/>
+      <c r="P234" s="33"/>
       <c r="BH234" s="21">
         <v>6.7027095434819522E-2</v>
       </c>
@@ -25473,8 +25473,8 @@
         <v>2.9322381930184807</v>
       </c>
       <c r="D235" s="28"/>
-      <c r="O235" s="36"/>
-      <c r="P235" s="36"/>
+      <c r="O235" s="33"/>
+      <c r="P235" s="33"/>
       <c r="BH235" s="21">
         <v>0.18166936576272241</v>
       </c>
@@ -25490,8 +25490,8 @@
         <v>3.1759069130732374</v>
       </c>
       <c r="D236" s="28"/>
-      <c r="O236" s="36"/>
-      <c r="P236" s="36"/>
+      <c r="O236" s="33"/>
+      <c r="P236" s="33"/>
       <c r="BH236" s="21">
         <v>8.2968760106616446E-4</v>
       </c>
@@ -25507,8 +25507,8 @@
         <v>3.5208761122518824</v>
       </c>
       <c r="D237" s="28"/>
-      <c r="O237" s="36"/>
-      <c r="P237" s="36"/>
+      <c r="O237" s="33"/>
+      <c r="P237" s="33"/>
       <c r="BH237" s="21">
         <v>7.3985599974694671E-3</v>
       </c>
@@ -25524,8 +25524,8 @@
         <v>3.7563312799452429</v>
       </c>
       <c r="D238" s="28"/>
-      <c r="O238" s="36"/>
-      <c r="P238" s="36"/>
+      <c r="O238" s="33"/>
+      <c r="P238" s="33"/>
       <c r="BH238" s="21">
         <v>4.0576557604792646E-2</v>
       </c>
@@ -25541,8 +25541,8 @@
         <v>4.0958247775496233</v>
       </c>
       <c r="D239" s="28"/>
-      <c r="O239" s="36"/>
-      <c r="P239" s="36"/>
+      <c r="O239" s="33"/>
+      <c r="P239" s="33"/>
       <c r="BH239" s="21">
         <v>8.0342936321758105E-4</v>
       </c>
@@ -25558,8 +25558,8 @@
         <v>0.24914442162902123</v>
       </c>
       <c r="D240" s="28"/>
-      <c r="O240" s="36"/>
-      <c r="P240" s="36"/>
+      <c r="O240" s="33"/>
+      <c r="P240" s="33"/>
       <c r="BH240" s="21">
         <v>2.2402077740333182</v>
       </c>
@@ -25575,8 +25575,8 @@
         <v>0.3613963039014374</v>
       </c>
       <c r="D241" s="28"/>
-      <c r="O241" s="36"/>
-      <c r="P241" s="36"/>
+      <c r="O241" s="33"/>
+      <c r="P241" s="33"/>
       <c r="BH241" s="21">
         <v>4.5270824061718837</v>
       </c>
@@ -25592,8 +25592,8 @@
         <v>0.47091033538672145</v>
       </c>
       <c r="D242" s="28"/>
-      <c r="O242" s="36"/>
-      <c r="P242" s="36"/>
+      <c r="O242" s="33"/>
+      <c r="P242" s="33"/>
       <c r="BH242" s="21">
         <v>5.3324586936767862</v>
       </c>
@@ -25609,8 +25609,8 @@
         <v>0.68446269678302529</v>
       </c>
       <c r="D243" s="28"/>
-      <c r="O243" s="36"/>
-      <c r="P243" s="36"/>
+      <c r="O243" s="33"/>
+      <c r="P243" s="33"/>
       <c r="BH243" s="21">
         <v>3.16111430435034</v>
       </c>
@@ -25626,8 +25626,8 @@
         <v>0.84052019164955505</v>
       </c>
       <c r="D244" s="28"/>
-      <c r="O244" s="36"/>
-      <c r="P244" s="36"/>
+      <c r="O244" s="33"/>
+      <c r="P244" s="33"/>
       <c r="BH244" s="21">
         <v>2.2421145654773214</v>
       </c>
@@ -25643,8 +25643,8 @@
         <v>1.6427104722792607</v>
       </c>
       <c r="D245" s="28"/>
-      <c r="O245" s="36"/>
-      <c r="P245" s="36"/>
+      <c r="O245" s="33"/>
+      <c r="P245" s="33"/>
       <c r="BH245" s="21">
         <v>0.47433514051772585</v>
       </c>
@@ -25660,8 +25660,8 @@
         <v>2.0314852840520192</v>
       </c>
       <c r="D246" s="28"/>
-      <c r="O246" s="36"/>
-      <c r="P246" s="36"/>
+      <c r="O246" s="33"/>
+      <c r="P246" s="33"/>
       <c r="BH246" s="21">
         <v>0.10094030205784604</v>
       </c>
@@ -25677,8 +25677,8 @@
         <v>2.1108829568788501</v>
       </c>
       <c r="D247" s="28"/>
-      <c r="O247" s="36"/>
-      <c r="P247" s="36"/>
+      <c r="O247" s="33"/>
+      <c r="P247" s="33"/>
       <c r="BH247" s="21">
         <v>0.19913247885824009</v>
       </c>
@@ -25694,8 +25694,8 @@
         <v>2.2450376454483232</v>
       </c>
       <c r="D248" s="28"/>
-      <c r="O248" s="36"/>
-      <c r="P248" s="36"/>
+      <c r="O248" s="33"/>
+      <c r="P248" s="33"/>
       <c r="BH248" s="21">
         <v>2.0176712233537311</v>
       </c>
@@ -25711,8 +25711,8 @@
         <v>2.3764544832306638</v>
       </c>
       <c r="D249" s="28"/>
-      <c r="O249" s="36"/>
-      <c r="P249" s="36"/>
+      <c r="O249" s="33"/>
+      <c r="P249" s="33"/>
       <c r="BH249" s="21">
         <v>3.1035203683652046</v>
       </c>
@@ -25728,8 +25728,8 @@
         <v>2.6064339493497606</v>
       </c>
       <c r="D250" s="28"/>
-      <c r="O250" s="36"/>
-      <c r="P250" s="36"/>
+      <c r="O250" s="33"/>
+      <c r="P250" s="33"/>
       <c r="BH250" s="21">
         <v>1.2559729903044137</v>
       </c>
@@ -25745,8 +25745,8 @@
         <v>2.9322381930184807</v>
       </c>
       <c r="D251" s="28"/>
-      <c r="O251" s="36"/>
-      <c r="P251" s="36"/>
+      <c r="O251" s="33"/>
+      <c r="P251" s="33"/>
       <c r="BH251" s="21">
         <v>0.43528950873451477</v>
       </c>
@@ -25762,8 +25762,8 @@
         <v>3.1759069130732374</v>
       </c>
       <c r="D252" s="28"/>
-      <c r="O252" s="36"/>
-      <c r="P252" s="36"/>
+      <c r="O252" s="33"/>
+      <c r="P252" s="33"/>
       <c r="BH252" s="21">
         <v>0.44975707102981433</v>
       </c>
@@ -25779,8 +25779,8 @@
         <v>3.5208761122518824</v>
       </c>
       <c r="D253" s="28"/>
-      <c r="O253" s="36"/>
-      <c r="P253" s="36"/>
+      <c r="O253" s="33"/>
+      <c r="P253" s="33"/>
       <c r="BH253" s="21">
         <v>0.33009040459632483</v>
       </c>
@@ -25796,8 +25796,8 @@
         <v>3.7563312799452429</v>
       </c>
       <c r="D254" s="28"/>
-      <c r="O254" s="36"/>
-      <c r="P254" s="36"/>
+      <c r="O254" s="33"/>
+      <c r="P254" s="33"/>
       <c r="BH254" s="21">
         <v>0.61933810363663644</v>
       </c>
@@ -25813,8 +25813,8 @@
         <v>4.0958247775496233</v>
       </c>
       <c r="D255" s="28"/>
-      <c r="O255" s="36"/>
-      <c r="P255" s="36"/>
+      <c r="O255" s="33"/>
+      <c r="P255" s="33"/>
       <c r="BH255" s="21">
         <v>0.10517262170754198</v>
       </c>
@@ -25830,8 +25830,8 @@
         <v>0.24914442162902123</v>
       </c>
       <c r="D256" s="28"/>
-      <c r="O256" s="36"/>
-      <c r="P256" s="36"/>
+      <c r="O256" s="33"/>
+      <c r="P256" s="33"/>
       <c r="BH256" s="21">
         <v>2.7071361606441093</v>
       </c>
@@ -25847,8 +25847,8 @@
         <v>0.3613963039014374</v>
       </c>
       <c r="D257" s="28"/>
-      <c r="O257" s="36"/>
-      <c r="P257" s="36"/>
+      <c r="O257" s="33"/>
+      <c r="P257" s="33"/>
       <c r="BH257" s="21">
         <v>3.5658683072262058</v>
       </c>
@@ -25864,8 +25864,8 @@
         <v>0.47091033538672145</v>
       </c>
       <c r="D258" s="28"/>
-      <c r="O258" s="36"/>
-      <c r="P258" s="36"/>
+      <c r="O258" s="33"/>
+      <c r="P258" s="33"/>
       <c r="BH258" s="21">
         <v>3.1045502950758488</v>
       </c>
@@ -25881,8 +25881,8 @@
         <v>0.84052019164955505</v>
       </c>
       <c r="D259" s="28"/>
-      <c r="O259" s="36"/>
-      <c r="P259" s="36"/>
+      <c r="O259" s="33"/>
+      <c r="P259" s="33"/>
       <c r="BH259" s="21">
         <v>2.3436297375993616</v>
       </c>
@@ -25898,8 +25898,8 @@
         <v>1.6427104722792607</v>
       </c>
       <c r="D260" s="28"/>
-      <c r="O260" s="36"/>
-      <c r="P260" s="36"/>
+      <c r="O260" s="33"/>
+      <c r="P260" s="33"/>
       <c r="BH260" s="21">
         <v>0.52128376577422708</v>
       </c>
@@ -25915,8 +25915,8 @@
         <v>2.0314852840520192</v>
       </c>
       <c r="D261" s="28"/>
-      <c r="O261" s="36"/>
-      <c r="P261" s="36"/>
+      <c r="O261" s="33"/>
+      <c r="P261" s="33"/>
       <c r="BH261" s="21">
         <v>0.65220436338273735</v>
       </c>
@@ -25932,8 +25932,8 @@
         <v>2.1108829568788501</v>
       </c>
       <c r="D262" s="28"/>
-      <c r="O262" s="36"/>
-      <c r="P262" s="36"/>
+      <c r="O262" s="33"/>
+      <c r="P262" s="33"/>
       <c r="BH262" s="21">
         <v>0.72653811030800075</v>
       </c>
@@ -25949,8 +25949,8 @@
         <v>2.2450376454483232</v>
       </c>
       <c r="D263" s="28"/>
-      <c r="O263" s="36"/>
-      <c r="P263" s="36"/>
+      <c r="O263" s="33"/>
+      <c r="P263" s="33"/>
       <c r="BH263" s="21">
         <v>1.9010029902286769</v>
       </c>
@@ -25966,8 +25966,8 @@
         <v>2.3764544832306638</v>
       </c>
       <c r="D264" s="28"/>
-      <c r="O264" s="36"/>
-      <c r="P264" s="36"/>
+      <c r="O264" s="33"/>
+      <c r="P264" s="33"/>
       <c r="BH264" s="21">
         <v>2.2628423596942753</v>
       </c>
@@ -25983,8 +25983,8 @@
         <v>2.6064339493497606</v>
       </c>
       <c r="D265" s="28"/>
-      <c r="O265" s="36"/>
-      <c r="P265" s="36"/>
+      <c r="O265" s="33"/>
+      <c r="P265" s="33"/>
       <c r="BH265" s="21">
         <v>1.3363237898911655</v>
       </c>
@@ -26000,8 +26000,8 @@
         <v>2.9322381930184807</v>
       </c>
       <c r="D266" s="28"/>
-      <c r="O266" s="36"/>
-      <c r="P266" s="36"/>
+      <c r="O266" s="33"/>
+      <c r="P266" s="33"/>
       <c r="BH266" s="21">
         <v>0.7415113449173163</v>
       </c>
@@ -26017,8 +26017,8 @@
         <v>3.1759069130732374</v>
       </c>
       <c r="D267" s="28"/>
-      <c r="O267" s="36"/>
-      <c r="P267" s="36"/>
+      <c r="O267" s="33"/>
+      <c r="P267" s="33"/>
       <c r="BH267" s="21">
         <v>0.57678704859443375</v>
       </c>
@@ -26034,8 +26034,8 @@
         <v>3.5208761122518824</v>
       </c>
       <c r="D268" s="28"/>
-      <c r="O268" s="36"/>
-      <c r="P268" s="36"/>
+      <c r="O268" s="33"/>
+      <c r="P268" s="33"/>
       <c r="BH268" s="21">
         <v>0.6491992359076123</v>
       </c>
@@ -26051,8 +26051,8 @@
         <v>3.7563312799452429</v>
       </c>
       <c r="D269" s="28"/>
-      <c r="O269" s="36"/>
-      <c r="P269" s="36"/>
+      <c r="O269" s="33"/>
+      <c r="P269" s="33"/>
       <c r="BH269" s="21">
         <v>1.1749373235460279</v>
       </c>
@@ -26068,8 +26068,8 @@
         <v>4.0958247775496233</v>
       </c>
       <c r="D270" s="28"/>
-      <c r="O270" s="36"/>
-      <c r="P270" s="36"/>
+      <c r="O270" s="33"/>
+      <c r="P270" s="33"/>
       <c r="BH270" s="21">
         <v>0.41992922457391135</v>
       </c>
@@ -26085,8 +26085,8 @@
         <v>0</v>
       </c>
       <c r="D271" s="28"/>
-      <c r="O271" s="36"/>
-      <c r="P271" s="36"/>
+      <c r="O271" s="33"/>
+      <c r="P271" s="33"/>
     </row>
     <row r="272" spans="1:60" s="21" customFormat="1" ht="15">
       <c r="A272" s="6" t="s">
@@ -26102,8 +26102,8 @@
       <c r="E272" s="21">
         <v>963</v>
       </c>
-      <c r="O272" s="36"/>
-      <c r="P272" s="36"/>
+      <c r="O272" s="33"/>
+      <c r="P272" s="33"/>
       <c r="AB272" s="21">
         <v>16.2</v>
       </c>
@@ -26134,8 +26134,8 @@
       <c r="E273" s="21">
         <v>938</v>
       </c>
-      <c r="O273" s="36"/>
-      <c r="P273" s="36"/>
+      <c r="O273" s="33"/>
+      <c r="P273" s="33"/>
       <c r="AB273" s="21">
         <v>16.399999999999999</v>
       </c>
@@ -26166,8 +26166,8 @@
       <c r="E274" s="21">
         <v>938</v>
       </c>
-      <c r="O274" s="36"/>
-      <c r="P274" s="36"/>
+      <c r="O274" s="33"/>
+      <c r="P274" s="33"/>
       <c r="AB274" s="21">
         <v>17.5</v>
       </c>
@@ -26198,8 +26198,8 @@
       <c r="E275" s="21">
         <v>913</v>
       </c>
-      <c r="O275" s="36"/>
-      <c r="P275" s="36"/>
+      <c r="O275" s="33"/>
+      <c r="P275" s="33"/>
       <c r="AB275" s="21">
         <v>19.600000000000001</v>
       </c>
@@ -26233,8 +26233,8 @@
       <c r="E276" s="21">
         <v>424</v>
       </c>
-      <c r="O276" s="36"/>
-      <c r="P276" s="36"/>
+      <c r="O276" s="33"/>
+      <c r="P276" s="33"/>
       <c r="AB276" s="21">
         <v>41</v>
       </c>
@@ -26265,8 +26265,8 @@
       <c r="E277" s="21">
         <v>888</v>
       </c>
-      <c r="O277" s="36"/>
-      <c r="P277" s="36"/>
+      <c r="O277" s="33"/>
+      <c r="P277" s="33"/>
       <c r="AB277" s="21">
         <v>15.7</v>
       </c>
@@ -26297,8 +26297,8 @@
       <c r="E278" s="21">
         <v>438</v>
       </c>
-      <c r="O278" s="36"/>
-      <c r="P278" s="36"/>
+      <c r="O278" s="33"/>
+      <c r="P278" s="33"/>
       <c r="AB278" s="21">
         <v>17.2</v>
       </c>
@@ -26329,8 +26329,8 @@
       <c r="E279" s="21">
         <v>438</v>
       </c>
-      <c r="O279" s="36"/>
-      <c r="P279" s="36"/>
+      <c r="O279" s="33"/>
+      <c r="P279" s="33"/>
       <c r="AB279" s="21">
         <v>19.399999999999999</v>
       </c>
@@ -26361,8 +26361,8 @@
       <c r="E280" s="21">
         <v>209</v>
       </c>
-      <c r="O280" s="36"/>
-      <c r="P280" s="36"/>
+      <c r="O280" s="33"/>
+      <c r="P280" s="33"/>
       <c r="AB280" s="21">
         <v>41</v>
       </c>
@@ -26398,8 +26398,8 @@
       <c r="E281" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O281" s="36"/>
-      <c r="P281" s="36"/>
+      <c r="O281" s="33"/>
+      <c r="P281" s="33"/>
     </row>
     <row r="282" spans="1:41" s="21" customFormat="1" ht="15">
       <c r="A282" s="6" t="s">
@@ -26417,8 +26417,8 @@
       <c r="E282" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O282" s="36"/>
-      <c r="P282" s="36"/>
+      <c r="O282" s="33"/>
+      <c r="P282" s="33"/>
       <c r="AF282" s="21">
         <v>108</v>
       </c>
@@ -26442,8 +26442,8 @@
       <c r="E283" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O283" s="36"/>
-      <c r="P283" s="36"/>
+      <c r="O283" s="33"/>
+      <c r="P283" s="33"/>
       <c r="AF283" s="21">
         <v>128.63999999999999</v>
       </c>
@@ -26467,8 +26467,8 @@
       <c r="E284" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O284" s="36"/>
-      <c r="P284" s="36"/>
+      <c r="O284" s="33"/>
+      <c r="P284" s="33"/>
       <c r="AF284" s="21">
         <v>168</v>
       </c>
@@ -26492,8 +26492,8 @@
       <c r="E285" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O285" s="36"/>
-      <c r="P285" s="36"/>
+      <c r="O285" s="33"/>
+      <c r="P285" s="33"/>
       <c r="AF285" s="21">
         <v>202.08</v>
       </c>
@@ -26520,8 +26520,8 @@
       <c r="F286" s="21">
         <v>8060.0000000000009</v>
       </c>
-      <c r="O286" s="36"/>
-      <c r="P286" s="36"/>
+      <c r="O286" s="33"/>
+      <c r="P286" s="33"/>
       <c r="Q286" s="21">
         <v>2680</v>
       </c>
@@ -26554,8 +26554,8 @@
       <c r="F287" s="21">
         <v>11060</v>
       </c>
-      <c r="O287" s="36"/>
-      <c r="P287" s="36"/>
+      <c r="O287" s="33"/>
+      <c r="P287" s="33"/>
       <c r="Q287" s="21">
         <v>2580</v>
       </c>
@@ -26588,8 +26588,8 @@
       <c r="F288" s="21">
         <v>12900</v>
       </c>
-      <c r="O288" s="36"/>
-      <c r="P288" s="36"/>
+      <c r="O288" s="33"/>
+      <c r="P288" s="33"/>
       <c r="Q288" s="21">
         <v>3040</v>
       </c>
@@ -26622,8 +26622,8 @@
       <c r="F289" s="21">
         <v>15000</v>
       </c>
-      <c r="O289" s="36"/>
-      <c r="P289" s="36"/>
+      <c r="O289" s="33"/>
+      <c r="P289" s="33"/>
       <c r="Q289" s="21">
         <v>4420</v>
       </c>
@@ -26653,8 +26653,8 @@
       <c r="E290" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O290" s="36"/>
-      <c r="P290" s="36"/>
+      <c r="O290" s="33"/>
+      <c r="P290" s="33"/>
       <c r="W290" s="21">
         <v>0.9</v>
       </c>
@@ -26678,8 +26678,8 @@
       <c r="E291" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O291" s="36"/>
-      <c r="P291" s="36"/>
+      <c r="O291" s="33"/>
+      <c r="P291" s="33"/>
       <c r="W291" s="21">
         <v>1.6</v>
       </c>
@@ -26703,8 +26703,8 @@
       <c r="E292" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O292" s="36"/>
-      <c r="P292" s="36"/>
+      <c r="O292" s="33"/>
+      <c r="P292" s="33"/>
       <c r="W292" s="21">
         <v>2.2999999999999998</v>
       </c>
@@ -26728,8 +26728,8 @@
       <c r="E293" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O293" s="36"/>
-      <c r="P293" s="36"/>
+      <c r="O293" s="33"/>
+      <c r="P293" s="33"/>
       <c r="W293" s="21">
         <v>1.3</v>
       </c>
@@ -26753,8 +26753,8 @@
       <c r="E294" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O294" s="36"/>
-      <c r="P294" s="36"/>
+      <c r="O294" s="33"/>
+      <c r="P294" s="33"/>
       <c r="W294" s="21">
         <v>2.2000000000000002</v>
       </c>
@@ -26778,8 +26778,8 @@
       <c r="E295" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O295" s="36"/>
-      <c r="P295" s="36"/>
+      <c r="O295" s="33"/>
+      <c r="P295" s="33"/>
       <c r="W295" s="21">
         <v>2.8</v>
       </c>
@@ -26803,8 +26803,8 @@
       <c r="E296" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O296" s="36"/>
-      <c r="P296" s="36"/>
+      <c r="O296" s="33"/>
+      <c r="P296" s="33"/>
       <c r="W296" s="21">
         <v>1.8</v>
       </c>
@@ -26828,8 +26828,8 @@
       <c r="E297" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O297" s="36"/>
-      <c r="P297" s="36"/>
+      <c r="O297" s="33"/>
+      <c r="P297" s="33"/>
       <c r="W297" s="21">
         <v>2.2000000000000002</v>
       </c>
@@ -26853,8 +26853,8 @@
       <c r="E298" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O298" s="36"/>
-      <c r="P298" s="36"/>
+      <c r="O298" s="33"/>
+      <c r="P298" s="33"/>
       <c r="W298" s="21">
         <v>3</v>
       </c>
@@ -26878,8 +26878,8 @@
       <c r="E299" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O299" s="36"/>
-      <c r="P299" s="36"/>
+      <c r="O299" s="33"/>
+      <c r="P299" s="33"/>
       <c r="W299" s="21">
         <v>2.2000000000000002</v>
       </c>
@@ -26903,8 +26903,8 @@
       <c r="E300" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O300" s="36"/>
-      <c r="P300" s="36"/>
+      <c r="O300" s="33"/>
+      <c r="P300" s="33"/>
       <c r="W300" s="21">
         <v>3.4</v>
       </c>
@@ -26928,8 +26928,8 @@
       <c r="E301" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O301" s="36"/>
-      <c r="P301" s="36"/>
+      <c r="O301" s="33"/>
+      <c r="P301" s="33"/>
       <c r="W301" s="21">
         <v>3.8</v>
       </c>
@@ -26956,8 +26956,8 @@
       <c r="F302" s="21">
         <v>21</v>
       </c>
-      <c r="O302" s="36"/>
-      <c r="P302" s="36"/>
+      <c r="O302" s="33"/>
+      <c r="P302" s="33"/>
     </row>
     <row r="303" spans="1:41" s="21" customFormat="1" ht="15">
       <c r="A303" s="6" t="s">
@@ -26978,8 +26978,8 @@
       <c r="F303" s="21">
         <v>97</v>
       </c>
-      <c r="O303" s="36"/>
-      <c r="P303" s="36"/>
+      <c r="O303" s="33"/>
+      <c r="P303" s="33"/>
     </row>
     <row r="304" spans="1:41" s="21" customFormat="1" ht="15">
       <c r="A304" s="6" t="s">
@@ -27000,8 +27000,8 @@
       <c r="F304" s="21">
         <v>138</v>
       </c>
-      <c r="O304" s="36"/>
-      <c r="P304" s="36"/>
+      <c r="O304" s="33"/>
+      <c r="P304" s="33"/>
     </row>
     <row r="305" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A305" s="6" t="s">
@@ -27022,8 +27022,8 @@
       <c r="F305" s="21">
         <v>179</v>
       </c>
-      <c r="O305" s="36"/>
-      <c r="P305" s="36"/>
+      <c r="O305" s="33"/>
+      <c r="P305" s="33"/>
     </row>
     <row r="306" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A306" s="6" t="s">
@@ -27044,8 +27044,8 @@
       <c r="F306" s="21">
         <v>281</v>
       </c>
-      <c r="O306" s="36"/>
-      <c r="P306" s="36"/>
+      <c r="O306" s="33"/>
+      <c r="P306" s="33"/>
     </row>
     <row r="307" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A307" s="6" t="s">
@@ -27066,8 +27066,8 @@
       <c r="F307" s="21">
         <v>348</v>
       </c>
-      <c r="O307" s="36"/>
-      <c r="P307" s="36"/>
+      <c r="O307" s="33"/>
+      <c r="P307" s="33"/>
     </row>
     <row r="308" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A308" s="6" t="s">
@@ -27088,8 +27088,8 @@
       <c r="F308" s="21">
         <v>432</v>
       </c>
-      <c r="O308" s="36"/>
-      <c r="P308" s="36"/>
+      <c r="O308" s="33"/>
+      <c r="P308" s="33"/>
     </row>
     <row r="309" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A309" s="6" t="s">
@@ -27110,8 +27110,8 @@
       <c r="F309" s="21">
         <v>560</v>
       </c>
-      <c r="O309" s="36"/>
-      <c r="P309" s="36"/>
+      <c r="O309" s="33"/>
+      <c r="P309" s="33"/>
     </row>
     <row r="310" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A310" s="6" t="s">
@@ -27132,8 +27132,8 @@
       <c r="F310" s="21">
         <v>772</v>
       </c>
-      <c r="O310" s="36"/>
-      <c r="P310" s="36"/>
+      <c r="O310" s="33"/>
+      <c r="P310" s="33"/>
     </row>
     <row r="311" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A311" s="6" t="s">
@@ -27154,10 +27154,10 @@
       <c r="F311" s="21">
         <v>891</v>
       </c>
-      <c r="O311" s="36">
+      <c r="O311" s="33">
         <v>191.28813559322032</v>
       </c>
-      <c r="P311" s="36">
+      <c r="P311" s="33">
         <v>30.20338983050847</v>
       </c>
       <c r="Q311" s="21">
@@ -27186,8 +27186,8 @@
       <c r="F312" s="21">
         <v>1577</v>
       </c>
-      <c r="O312" s="36"/>
-      <c r="P312" s="36"/>
+      <c r="O312" s="33"/>
+      <c r="P312" s="33"/>
     </row>
     <row r="313" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A313" s="6" t="s">
@@ -27208,10 +27208,10 @@
       <c r="F313" s="21">
         <v>2572</v>
       </c>
-      <c r="O313" s="36">
+      <c r="O313" s="33">
         <v>482.58144329896908</v>
       </c>
-      <c r="P313" s="36">
+      <c r="P313" s="33">
         <v>10.606185567010309</v>
       </c>
       <c r="Q313" s="21">
@@ -27240,8 +27240,8 @@
       <c r="F314" s="21">
         <v>3420.0000000000005</v>
       </c>
-      <c r="O314" s="36"/>
-      <c r="P314" s="36"/>
+      <c r="O314" s="33"/>
+      <c r="P314" s="33"/>
     </row>
     <row r="315" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A315" s="6" t="s">
@@ -27262,8 +27262,8 @@
       <c r="F315" s="21">
         <v>3929</v>
       </c>
-      <c r="O315" s="36"/>
-      <c r="P315" s="36"/>
+      <c r="O315" s="33"/>
+      <c r="P315" s="33"/>
     </row>
     <row r="316" spans="1:22" s="21" customFormat="1" ht="15">
       <c r="A316" s="6" t="s">
@@ -27302,8 +27302,8 @@
       <c r="N316" s="21">
         <v>350</v>
       </c>
-      <c r="O316" s="36"/>
-      <c r="P316" s="36"/>
+      <c r="O316" s="33"/>
+      <c r="P316" s="33"/>
       <c r="S316" s="21">
         <v>2160.0021600021601</v>
       </c>
@@ -27345,8 +27345,8 @@
       <c r="N317" s="21">
         <v>260</v>
       </c>
-      <c r="O317" s="36"/>
-      <c r="P317" s="36"/>
+      <c r="O317" s="33"/>
+      <c r="P317" s="33"/>
       <c r="S317" s="21">
         <v>1530.0015300015302</v>
       </c>
@@ -27388,8 +27388,8 @@
       <c r="N318" s="21">
         <v>160</v>
       </c>
-      <c r="O318" s="36"/>
-      <c r="P318" s="36"/>
+      <c r="O318" s="33"/>
+      <c r="P318" s="33"/>
       <c r="S318" s="21">
         <v>900.00090000090006</v>
       </c>
@@ -27431,8 +27431,8 @@
       <c r="N319" s="21">
         <v>100</v>
       </c>
-      <c r="O319" s="36"/>
-      <c r="P319" s="36"/>
+      <c r="O319" s="33"/>
+      <c r="P319" s="33"/>
       <c r="S319" s="21">
         <v>540.00054000054001</v>
       </c>
@@ -27474,8 +27474,8 @@
       <c r="N320" s="21">
         <v>2080</v>
       </c>
-      <c r="O320" s="36"/>
-      <c r="P320" s="36"/>
+      <c r="O320" s="33"/>
+      <c r="P320" s="33"/>
       <c r="S320" s="21">
         <v>15120.015120015123</v>
       </c>
@@ -27523,8 +27523,8 @@
       <c r="N321" s="21">
         <v>1260</v>
       </c>
-      <c r="O321" s="36"/>
-      <c r="P321" s="36"/>
+      <c r="O321" s="33"/>
+      <c r="P321" s="33"/>
       <c r="S321" s="21">
         <v>9270.00927000927</v>
       </c>
@@ -27572,8 +27572,8 @@
       <c r="N322" s="21">
         <v>990</v>
       </c>
-      <c r="O322" s="36"/>
-      <c r="P322" s="36"/>
+      <c r="O322" s="33"/>
+      <c r="P322" s="33"/>
       <c r="S322" s="21">
         <v>6570.0065700065697</v>
       </c>
@@ -27621,8 +27621,8 @@
       <c r="N323" s="21">
         <v>690</v>
       </c>
-      <c r="O323" s="36"/>
-      <c r="P323" s="36"/>
+      <c r="O323" s="33"/>
+      <c r="P323" s="33"/>
       <c r="S323" s="21">
         <v>4860.0048600048603</v>
       </c>
@@ -27644,8 +27644,8 @@
         <v>0</v>
       </c>
       <c r="D324" s="28"/>
-      <c r="O324" s="36"/>
-      <c r="P324" s="36"/>
+      <c r="O324" s="33"/>
+      <c r="P324" s="33"/>
       <c r="AF324" s="21">
         <v>0</v>
       </c>
@@ -28282,9 +28282,9 @@
         <v>3.8960448710472115</v>
       </c>
       <c r="D365" s="28"/>
-      <c r="F365" s="37"/>
-      <c r="O365" s="34"/>
-      <c r="P365" s="34"/>
+      <c r="F365" s="34"/>
+      <c r="O365" s="31"/>
+      <c r="P365" s="31"/>
       <c r="AB365" s="21">
         <v>10.89</v>
       </c>
@@ -28303,8 +28303,8 @@
         <v>5.2020275860784976E-2</v>
       </c>
       <c r="D366" s="28"/>
-      <c r="O366" s="34"/>
-      <c r="P366" s="34"/>
+      <c r="O366" s="31"/>
+      <c r="P366" s="31"/>
       <c r="AB366" s="21">
         <v>0.31</v>
       </c>
@@ -28320,8 +28320,8 @@
         <v>0.34223865697884853</v>
       </c>
       <c r="D367" s="28"/>
-      <c r="O367" s="34"/>
-      <c r="P367" s="34"/>
+      <c r="O367" s="31"/>
+      <c r="P367" s="31"/>
       <c r="AB367" s="21">
         <v>0.72</v>
       </c>
@@ -28337,8 +28337,8 @@
         <v>0.72554595279515888</v>
       </c>
       <c r="D368" s="28"/>
-      <c r="O368" s="34"/>
-      <c r="P368" s="34"/>
+      <c r="O368" s="31"/>
+      <c r="P368" s="31"/>
       <c r="AB368" s="21">
         <v>0.91</v>
       </c>
@@ -28354,8 +28354,8 @@
         <v>0.81863486749340564</v>
       </c>
       <c r="D369" s="28"/>
-      <c r="O369" s="34"/>
-      <c r="P369" s="34"/>
+      <c r="O369" s="31"/>
+      <c r="P369" s="31"/>
       <c r="AB369" s="21">
         <v>0.94</v>
       </c>
@@ -28371,8 +28371,8 @@
         <v>0.91993750995914481</v>
       </c>
       <c r="D370" s="28"/>
-      <c r="O370" s="34"/>
-      <c r="P370" s="34"/>
+      <c r="O370" s="31"/>
+      <c r="P370" s="31"/>
       <c r="AB370" s="21">
         <v>0.98</v>
       </c>
@@ -28386,8 +28386,8 @@
         <v>1.00755060614573</v>
       </c>
       <c r="D371" s="28"/>
-      <c r="O371" s="34"/>
-      <c r="P371" s="34"/>
+      <c r="O371" s="31"/>
+      <c r="P371" s="31"/>
     </row>
     <row r="372" spans="1:29" s="21" customFormat="1" ht="15">
       <c r="A372" s="19" t="s">
@@ -28400,8 +28400,8 @@
         <v>1.0896878838206536</v>
       </c>
       <c r="D372" s="28"/>
-      <c r="O372" s="34"/>
-      <c r="P372" s="34"/>
+      <c r="O372" s="31"/>
+      <c r="P372" s="31"/>
       <c r="AB372" s="21">
         <v>1.24</v>
       </c>
@@ -28417,8 +28417,8 @@
         <v>1.149921887448931</v>
       </c>
       <c r="D373" s="28"/>
-      <c r="O373" s="34"/>
-      <c r="P373" s="34"/>
+      <c r="O373" s="31"/>
+      <c r="P373" s="31"/>
       <c r="AB373" s="21">
         <v>1.47</v>
       </c>
@@ -28434,8 +28434,8 @@
         <v>1.243010802147178</v>
       </c>
       <c r="D374" s="28"/>
-      <c r="O374" s="34"/>
-      <c r="P374" s="34"/>
+      <c r="O374" s="31"/>
+      <c r="P374" s="31"/>
       <c r="AB374" s="21">
         <v>1.77</v>
       </c>
@@ -28451,8 +28451,8 @@
         <v>1.3196722613104399</v>
       </c>
       <c r="D375" s="28"/>
-      <c r="O375" s="34"/>
-      <c r="P375" s="34"/>
+      <c r="O375" s="31"/>
+      <c r="P375" s="31"/>
       <c r="AB375" s="21">
         <v>2.0499999999999998</v>
       </c>
@@ -28468,8 +28468,8 @@
         <v>1.3990716297295327</v>
       </c>
       <c r="D376" s="28"/>
-      <c r="O376" s="34"/>
-      <c r="P376" s="34"/>
+      <c r="O376" s="31"/>
+      <c r="P376" s="31"/>
       <c r="AB376" s="21">
         <v>2.4</v>
       </c>
@@ -28483,8 +28483,8 @@
         <v>1.4948984536836103</v>
       </c>
       <c r="D377" s="28"/>
-      <c r="O377" s="34"/>
-      <c r="P377" s="34"/>
+      <c r="O377" s="31"/>
+      <c r="P377" s="31"/>
     </row>
     <row r="378" spans="1:29" s="21" customFormat="1" ht="15">
       <c r="A378" s="19" t="s">
@@ -28497,8 +28497,8 @@
         <v>1.5879873683818573</v>
       </c>
       <c r="D378" s="28"/>
-      <c r="O378" s="34"/>
-      <c r="P378" s="34"/>
+      <c r="O378" s="31"/>
+      <c r="P378" s="31"/>
       <c r="AB378" s="21">
         <v>2.84</v>
       </c>
@@ -28514,8 +28514,8 @@
         <v>1.7659514700108585</v>
       </c>
       <c r="D379" s="28"/>
-      <c r="O379" s="34"/>
-      <c r="P379" s="34"/>
+      <c r="O379" s="31"/>
+      <c r="P379" s="31"/>
       <c r="AB379" s="21">
         <v>2.93</v>
       </c>
@@ -28531,8 +28531,8 @@
         <v>1.9685567549423368</v>
       </c>
       <c r="D380" s="28"/>
-      <c r="O380" s="34"/>
-      <c r="P380" s="34"/>
+      <c r="O380" s="31"/>
+      <c r="P380" s="31"/>
       <c r="AB380" s="21">
         <v>2.92</v>
       </c>
@@ -28548,8 +28548,8 @@
         <v>2.094500580710553</v>
       </c>
       <c r="D381" s="28"/>
-      <c r="O381" s="34"/>
-      <c r="P381" s="34"/>
+      <c r="O381" s="31"/>
+      <c r="P381" s="31"/>
       <c r="AB381" s="21">
         <v>3.24</v>
       </c>
@@ -28568,8 +28568,8 @@
         <v>2.1930653139204614</v>
       </c>
       <c r="D382" s="28"/>
-      <c r="O382" s="34"/>
-      <c r="P382" s="34"/>
+      <c r="O382" s="31"/>
+      <c r="P382" s="31"/>
       <c r="AB382" s="21">
         <v>3.64</v>
       </c>
@@ -28588,8 +28588,8 @@
         <v>2.288892137874539</v>
       </c>
       <c r="D383" s="28"/>
-      <c r="O383" s="34"/>
-      <c r="P383" s="34"/>
+      <c r="O383" s="31"/>
+      <c r="P383" s="31"/>
       <c r="AB383" s="21">
         <v>4.32</v>
       </c>
@@ -28608,8 +28608,8 @@
         <v>2.3929326895961087</v>
       </c>
       <c r="D384" s="28"/>
-      <c r="O384" s="34"/>
-      <c r="P384" s="34"/>
+      <c r="O384" s="31"/>
+      <c r="P384" s="31"/>
       <c r="AB384" s="21">
         <v>4.8899999999999997</v>
       </c>
@@ -28628,8 +28628,8 @@
         <v>2.4805457857826942</v>
       </c>
       <c r="D385" s="28"/>
-      <c r="O385" s="34"/>
-      <c r="P385" s="34"/>
+      <c r="O385" s="31"/>
+      <c r="P385" s="31"/>
       <c r="AB385" s="21">
         <v>5.25</v>
       </c>
@@ -28648,8 +28648,8 @@
         <v>2.5517314264342947</v>
       </c>
       <c r="D386" s="28"/>
-      <c r="O386" s="34"/>
-      <c r="P386" s="34"/>
+      <c r="O386" s="31"/>
+      <c r="P386" s="31"/>
       <c r="AB386" s="21">
         <v>5.57</v>
       </c>
@@ -28666,8 +28666,8 @@
         <v>2.6475582503883723</v>
       </c>
       <c r="D387" s="28"/>
-      <c r="O387" s="34"/>
-      <c r="P387" s="34"/>
+      <c r="O387" s="31"/>
+      <c r="P387" s="31"/>
       <c r="AC387" s="21">
         <v>8.36</v>
       </c>
@@ -28683,8 +28683,8 @@
         <v>2.8748047186223276</v>
       </c>
       <c r="D388" s="28"/>
-      <c r="O388" s="34"/>
-      <c r="P388" s="34"/>
+      <c r="O388" s="31"/>
+      <c r="P388" s="31"/>
       <c r="AB388" s="21">
         <v>5.95</v>
       </c>
@@ -28703,8 +28703,8 @@
         <v>3.1239544609029295</v>
       </c>
       <c r="D389" s="28"/>
-      <c r="O389" s="34"/>
-      <c r="P389" s="34"/>
+      <c r="O389" s="31"/>
+      <c r="P389" s="31"/>
       <c r="AB389" s="21">
         <v>6.11</v>
       </c>
@@ -28723,8 +28723,8 @@
         <v>3.2991806532760997</v>
       </c>
       <c r="D390" s="28"/>
-      <c r="O390" s="34"/>
-      <c r="P390" s="34"/>
+      <c r="O390" s="31"/>
+      <c r="P390" s="31"/>
       <c r="AB390" s="21">
         <v>6.52</v>
       </c>
@@ -28743,8 +28743,8 @@
         <v>3.4689310271376086</v>
       </c>
       <c r="D391" s="28"/>
-      <c r="O391" s="34"/>
-      <c r="P391" s="34"/>
+      <c r="O391" s="31"/>
+      <c r="P391" s="31"/>
       <c r="AB391" s="21">
         <v>7.36</v>
       </c>
@@ -28763,8 +28763,8 @@
         <v>3.6222539454641329</v>
       </c>
       <c r="D392" s="28"/>
-      <c r="O392" s="34"/>
-      <c r="P392" s="34"/>
+      <c r="O392" s="31"/>
+      <c r="P392" s="31"/>
       <c r="AB392" s="21">
         <v>8.35</v>
       </c>
@@ -28783,8 +28783,8 @@
         <v>3.8960448710472115</v>
       </c>
       <c r="D393" s="28"/>
-      <c r="O393" s="34"/>
-      <c r="P393" s="34"/>
+      <c r="O393" s="31"/>
+      <c r="P393" s="31"/>
       <c r="AB393" s="21">
         <v>8.67</v>
       </c>
@@ -28808,8 +28808,8 @@
       <c r="E394" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O394" s="34"/>
-      <c r="P394" s="34"/>
+      <c r="O394" s="31"/>
+      <c r="P394" s="31"/>
       <c r="AB394" s="21">
         <v>4.81395348837209</v>
       </c>
@@ -28833,8 +28833,8 @@
       <c r="E395" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O395" s="34"/>
-      <c r="P395" s="34"/>
+      <c r="O395" s="31"/>
+      <c r="P395" s="31"/>
       <c r="AB395" s="21">
         <v>4.81395348837209</v>
       </c>
@@ -28858,8 +28858,8 @@
       <c r="E396" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O396" s="34"/>
-      <c r="P396" s="34"/>
+      <c r="O396" s="31"/>
+      <c r="P396" s="31"/>
       <c r="AB396" s="21">
         <v>6.9069767441860499</v>
       </c>
@@ -28883,8 +28883,8 @@
       <c r="E397" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O397" s="34"/>
-      <c r="P397" s="34"/>
+      <c r="O397" s="31"/>
+      <c r="P397" s="31"/>
       <c r="AB397" s="21">
         <v>9.3488372093023209</v>
       </c>
@@ -28908,8 +28908,8 @@
       <c r="E398" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O398" s="34"/>
-      <c r="P398" s="34"/>
+      <c r="O398" s="31"/>
+      <c r="P398" s="31"/>
       <c r="AB398" s="21">
         <v>10.5348837209302</v>
       </c>
@@ -28933,8 +28933,8 @@
       <c r="E399" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O399" s="34"/>
-      <c r="P399" s="34"/>
+      <c r="O399" s="31"/>
+      <c r="P399" s="31"/>
       <c r="AB399" s="21">
         <v>11.0930232558139</v>
       </c>
@@ -28958,8 +28958,8 @@
       <c r="E400" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O400" s="34"/>
-      <c r="P400" s="34"/>
+      <c r="O400" s="31"/>
+      <c r="P400" s="31"/>
       <c r="AB400" s="21">
         <v>11.7209302325581</v>
       </c>
@@ -28983,9 +28983,9 @@
       <c r="E401" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="F401" s="37"/>
-      <c r="O401" s="34"/>
-      <c r="P401" s="34"/>
+      <c r="F401" s="34"/>
+      <c r="O401" s="31"/>
+      <c r="P401" s="31"/>
       <c r="Q401" s="21">
         <v>247.74774774774701</v>
       </c>
@@ -29012,8 +29012,8 @@
       <c r="E402" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O402" s="34"/>
-      <c r="P402" s="34"/>
+      <c r="O402" s="31"/>
+      <c r="P402" s="31"/>
       <c r="AC402" s="21">
         <v>8.6666411746711507</v>
       </c>
@@ -29034,8 +29034,8 @@
       <c r="E403" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O403" s="34"/>
-      <c r="P403" s="34"/>
+      <c r="O403" s="31"/>
+      <c r="P403" s="31"/>
       <c r="AB403" s="21">
         <v>12.1395348837209</v>
       </c>
@@ -29059,8 +29059,8 @@
       <c r="E404" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O404" s="34"/>
-      <c r="P404" s="34"/>
+      <c r="O404" s="31"/>
+      <c r="P404" s="31"/>
       <c r="AB404" s="21">
         <v>13.5348837209302</v>
       </c>
@@ -29084,8 +29084,8 @@
       <c r="E405" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O405" s="34"/>
-      <c r="P405" s="34"/>
+      <c r="O405" s="31"/>
+      <c r="P405" s="31"/>
       <c r="AB405" s="21">
         <v>15.279069767441801</v>
       </c>
@@ -29109,8 +29109,8 @@
       <c r="E406" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O406" s="34"/>
-      <c r="P406" s="34"/>
+      <c r="O406" s="31"/>
+      <c r="P406" s="31"/>
       <c r="AB406" s="21">
         <v>16.1860465116279</v>
       </c>
@@ -29134,8 +29134,8 @@
       <c r="E407" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O407" s="34"/>
-      <c r="P407" s="34"/>
+      <c r="O407" s="31"/>
+      <c r="P407" s="31"/>
       <c r="AB407" s="21">
         <v>17.023255813953401</v>
       </c>
@@ -29159,8 +29159,8 @@
       <c r="E408" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O408" s="34"/>
-      <c r="P408" s="34"/>
+      <c r="O408" s="31"/>
+      <c r="P408" s="31"/>
       <c r="AB408" s="21">
         <v>18</v>
       </c>
@@ -29184,8 +29184,8 @@
       <c r="E409" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O409" s="34"/>
-      <c r="P409" s="34"/>
+      <c r="O409" s="31"/>
+      <c r="P409" s="31"/>
       <c r="AB409" s="21">
         <v>18.0697674418604</v>
       </c>
@@ -29209,8 +29209,8 @@
       <c r="E410" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O410" s="34"/>
-      <c r="P410" s="34"/>
+      <c r="O410" s="31"/>
+      <c r="P410" s="31"/>
       <c r="Q410" s="21">
         <v>803.30330330330264</v>
       </c>
@@ -29237,8 +29237,8 @@
       <c r="E411" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O411" s="34"/>
-      <c r="P411" s="34"/>
+      <c r="O411" s="31"/>
+      <c r="P411" s="31"/>
       <c r="AB411" s="21">
         <v>18.906976744186</v>
       </c>
@@ -29262,8 +29262,8 @@
       <c r="E412" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O412" s="34"/>
-      <c r="P412" s="34"/>
+      <c r="O412" s="31"/>
+      <c r="P412" s="31"/>
       <c r="AB412" s="21">
         <v>21.209302325581302</v>
       </c>
@@ -29287,8 +29287,8 @@
       <c r="E413" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O413" s="34"/>
-      <c r="P413" s="34"/>
+      <c r="O413" s="31"/>
+      <c r="P413" s="31"/>
       <c r="AB413" s="21">
         <v>21.697674418604599</v>
       </c>
@@ -29312,8 +29312,8 @@
       <c r="E414" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O414" s="34"/>
-      <c r="P414" s="34"/>
+      <c r="O414" s="31"/>
+      <c r="P414" s="31"/>
       <c r="AB414" s="21">
         <v>21.767441860465102</v>
       </c>
@@ -29337,8 +29337,8 @@
       <c r="E415" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O415" s="34"/>
-      <c r="P415" s="34"/>
+      <c r="O415" s="31"/>
+      <c r="P415" s="31"/>
       <c r="AB415" s="21">
         <v>21.906976744186</v>
       </c>
@@ -29362,8 +29362,8 @@
       <c r="E416" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O416" s="34"/>
-      <c r="P416" s="34"/>
+      <c r="O416" s="31"/>
+      <c r="P416" s="31"/>
       <c r="AB416" s="21">
         <v>21.906976744186</v>
       </c>
@@ -29387,8 +29387,8 @@
       <c r="E417" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O417" s="34"/>
-      <c r="P417" s="34"/>
+      <c r="O417" s="31"/>
+      <c r="P417" s="31"/>
       <c r="AB417" s="21">
         <v>22.2558139534883</v>
       </c>
@@ -29412,8 +29412,8 @@
       <c r="E418" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O418" s="34"/>
-      <c r="P418" s="34"/>
+      <c r="O418" s="31"/>
+      <c r="P418" s="31"/>
       <c r="AB418" s="21">
         <v>22.5348837209302</v>
       </c>
@@ -29437,8 +29437,8 @@
       <c r="E419" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O419" s="34"/>
-      <c r="P419" s="34"/>
+      <c r="O419" s="31"/>
+      <c r="P419" s="31"/>
       <c r="AB419" s="21">
         <v>22.5348837209302</v>
       </c>
@@ -29462,8 +29462,8 @@
       <c r="E420" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O420" s="34"/>
-      <c r="P420" s="34"/>
+      <c r="O420" s="31"/>
+      <c r="P420" s="31"/>
       <c r="AB420" s="21">
         <v>22.813953488372</v>
       </c>
@@ -29487,8 +29487,8 @@
       <c r="E421" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O421" s="34"/>
-      <c r="P421" s="34"/>
+      <c r="O421" s="31"/>
+      <c r="P421" s="31"/>
       <c r="AB421" s="21">
         <v>23.023255813953401</v>
       </c>
@@ -29512,8 +29512,8 @@
       <c r="E422" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O422" s="34"/>
-      <c r="P422" s="34"/>
+      <c r="O422" s="31"/>
+      <c r="P422" s="31"/>
       <c r="AB422" s="21">
         <v>23.0930232558139</v>
       </c>
@@ -29537,8 +29537,8 @@
       <c r="E423" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O423" s="34"/>
-      <c r="P423" s="34"/>
+      <c r="O423" s="31"/>
+      <c r="P423" s="31"/>
       <c r="Q423" s="21">
         <v>1227.4774774774701</v>
       </c>
@@ -29565,8 +29565,8 @@
       <c r="E424" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O424" s="34"/>
-      <c r="P424" s="34"/>
+      <c r="O424" s="31"/>
+      <c r="P424" s="31"/>
       <c r="AC424" s="21">
         <v>14.0769348424594</v>
       </c>
@@ -29587,8 +29587,8 @@
       <c r="E425" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O425" s="34"/>
-      <c r="P425" s="34"/>
+      <c r="O425" s="31"/>
+      <c r="P425" s="31"/>
       <c r="AC425" s="21">
         <v>14.278927041908799</v>
       </c>
@@ -29609,8 +29609,8 @@
       <c r="E426" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O426" s="34"/>
-      <c r="P426" s="34"/>
+      <c r="O426" s="31"/>
+      <c r="P426" s="31"/>
       <c r="AB426" s="21">
         <v>23.790697674418599</v>
       </c>
@@ -29634,8 +29634,8 @@
       <c r="E427" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O427" s="34"/>
-      <c r="P427" s="34"/>
+      <c r="O427" s="31"/>
+      <c r="P427" s="31"/>
       <c r="AB427" s="21">
         <v>23.581395348837201</v>
       </c>
@@ -29659,8 +29659,8 @@
       <c r="E428" s="21">
         <v>1111.1099999999999</v>
       </c>
-      <c r="O428" s="34"/>
-      <c r="P428" s="34"/>
+      <c r="O428" s="31"/>
+      <c r="P428" s="31"/>
       <c r="AB428" s="21">
         <v>24.209302325581302</v>
       </c>
@@ -52190,9 +52190,6 @@
       <c r="AI1227" s="21">
         <v>1.44</v>
       </c>
-      <c r="AJ1227" s="21">
-        <v>87676.027777777796</v>
-      </c>
     </row>
     <row r="1228" spans="1:67" s="21" customFormat="1">
       <c r="A1228" s="19" t="s">
@@ -52249,9 +52246,6 @@
       <c r="AI1228" s="21">
         <v>13.25</v>
       </c>
-      <c r="AJ1228" s="21">
-        <v>46286.473029045643</v>
-      </c>
     </row>
     <row r="1229" spans="1:67" s="21" customFormat="1">
       <c r="A1229" s="19" t="s">
@@ -52308,9 +52302,6 @@
       <c r="AI1229" s="21">
         <v>22.83</v>
       </c>
-      <c r="AJ1229" s="21">
-        <v>47189.004964953267</v>
-      </c>
     </row>
     <row r="1230" spans="1:67" s="21" customFormat="1">
       <c r="A1230" s="19" t="s">
@@ -52367,9 +52358,6 @@
       <c r="AI1230" s="21">
         <v>24.42</v>
       </c>
-      <c r="AJ1230" s="21">
-        <v>61916.403296815792</v>
-      </c>
     </row>
     <row r="1231" spans="1:67" s="21" customFormat="1">
       <c r="A1231" s="19" t="s">
@@ -52426,9 +52414,6 @@
       <c r="AI1231" s="21">
         <v>30.74</v>
       </c>
-      <c r="AJ1231" s="21">
-        <v>55662.544247787613</v>
-      </c>
     </row>
     <row r="1232" spans="1:67" s="21" customFormat="1">
       <c r="A1232" s="19" t="s">
@@ -52485,11 +52470,8 @@
       <c r="AI1232" s="21">
         <v>31.42</v>
       </c>
-      <c r="AJ1232" s="21">
-        <v>52931.843640606756</v>
-      </c>
-    </row>
-    <row r="1233" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1233" spans="1:35" s="21" customFormat="1">
       <c r="A1233" s="19" t="s">
         <v>178</v>
       </c>
@@ -52503,7 +52485,7 @@
         <v>226.69</v>
       </c>
     </row>
-    <row r="1234" spans="1:36" s="21" customFormat="1">
+    <row r="1234" spans="1:35" s="21" customFormat="1">
       <c r="A1234" s="19" t="s">
         <v>178</v>
       </c>
@@ -52517,7 +52499,7 @@
         <v>263.12</v>
       </c>
     </row>
-    <row r="1235" spans="1:36" s="21" customFormat="1">
+    <row r="1235" spans="1:35" s="21" customFormat="1">
       <c r="A1235" s="19" t="s">
         <v>178</v>
       </c>
@@ -52531,7 +52513,7 @@
         <v>301.10000000000002</v>
       </c>
     </row>
-    <row r="1236" spans="1:36" s="21" customFormat="1">
+    <row r="1236" spans="1:35" s="21" customFormat="1">
       <c r="A1236" s="19" t="s">
         <v>178</v>
       </c>
@@ -52545,7 +52527,7 @@
         <v>315.02</v>
       </c>
     </row>
-    <row r="1237" spans="1:36" s="21" customFormat="1">
+    <row r="1237" spans="1:35" s="21" customFormat="1">
       <c r="A1237" s="19" t="s">
         <v>179</v>
       </c>
@@ -52600,11 +52582,8 @@
       <c r="AI1237" s="21">
         <v>2.19</v>
       </c>
-      <c r="AJ1237" s="21">
-        <v>95179.908675799103</v>
-      </c>
-    </row>
-    <row r="1238" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1238" spans="1:35" s="21" customFormat="1">
       <c r="A1238" s="19" t="s">
         <v>179</v>
       </c>
@@ -52659,11 +52638,8 @@
       <c r="AI1238" s="21">
         <v>20.92</v>
       </c>
-      <c r="AJ1238" s="21">
-        <v>47723.455675029865</v>
-      </c>
-    </row>
-    <row r="1239" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1239" spans="1:35" s="21" customFormat="1">
       <c r="A1239" s="19" t="s">
         <v>179</v>
       </c>
@@ -52718,11 +52694,8 @@
       <c r="AI1239" s="21">
         <v>33.909999999999997</v>
       </c>
-      <c r="AJ1239" s="21">
-        <v>44098.253612503679</v>
-      </c>
-    </row>
-    <row r="1240" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1240" spans="1:35" s="21" customFormat="1">
       <c r="A1240" s="19" t="s">
         <v>179</v>
       </c>
@@ -52777,11 +52750,8 @@
       <c r="AI1240" s="21">
         <v>36.270000000000003</v>
       </c>
-      <c r="AJ1240" s="21">
-        <v>58169.059829059828</v>
-      </c>
-    </row>
-    <row r="1241" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1241" spans="1:35" s="21" customFormat="1">
       <c r="A1241" s="19" t="s">
         <v>179</v>
       </c>
@@ -52836,11 +52806,8 @@
       <c r="AI1241" s="21">
         <v>39.31</v>
       </c>
-      <c r="AJ1241" s="21">
-        <v>56864.448175851016</v>
-      </c>
-    </row>
-    <row r="1242" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1242" spans="1:35" s="21" customFormat="1">
       <c r="A1242" s="19" t="s">
         <v>179</v>
       </c>
@@ -52895,11 +52862,8 @@
       <c r="AI1242" s="21">
         <v>45.2</v>
       </c>
-      <c r="AJ1242" s="21">
-        <v>53875.654546795486</v>
-      </c>
-    </row>
-    <row r="1243" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1243" spans="1:35" s="21" customFormat="1">
       <c r="A1243" s="19" t="s">
         <v>179</v>
       </c>
@@ -52913,7 +52877,7 @@
         <v>251.86</v>
       </c>
     </row>
-    <row r="1244" spans="1:36" s="21" customFormat="1">
+    <row r="1244" spans="1:35" s="21" customFormat="1">
       <c r="A1244" s="19" t="s">
         <v>179</v>
       </c>
@@ -52927,7 +52891,7 @@
         <v>271.58</v>
       </c>
     </row>
-    <row r="1245" spans="1:36" s="21" customFormat="1">
+    <row r="1245" spans="1:35" s="21" customFormat="1">
       <c r="A1245" s="19" t="s">
         <v>179</v>
       </c>
@@ -52941,7 +52905,7 @@
         <v>308.68</v>
       </c>
     </row>
-    <row r="1246" spans="1:36" s="21" customFormat="1">
+    <row r="1246" spans="1:35" s="21" customFormat="1">
       <c r="A1246" s="19" t="s">
         <v>179</v>
       </c>
@@ -52955,7 +52919,7 @@
         <v>325.72000000000003</v>
       </c>
     </row>
-    <row r="1247" spans="1:36" s="21" customFormat="1">
+    <row r="1247" spans="1:35" s="21" customFormat="1">
       <c r="A1247" s="19" t="s">
         <v>180</v>
       </c>
@@ -53010,11 +52974,8 @@
       <c r="AI1247" s="21">
         <v>0.33</v>
       </c>
-      <c r="AJ1247" s="21">
-        <v>170888.12121212122</v>
-      </c>
-    </row>
-    <row r="1248" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1248" spans="1:35" s="21" customFormat="1">
       <c r="A1248" s="19" t="s">
         <v>180</v>
       </c>
@@ -53069,11 +53030,8 @@
       <c r="AI1248" s="21">
         <v>7.8</v>
       </c>
-      <c r="AJ1248" s="21">
-        <v>48020.615384615383</v>
-      </c>
-    </row>
-    <row r="1249" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1249" spans="1:35" s="21" customFormat="1">
       <c r="A1249" s="19" t="s">
         <v>180</v>
       </c>
@@ -53128,11 +53086,8 @@
       <c r="AI1249" s="21">
         <v>13.38</v>
       </c>
-      <c r="AJ1249" s="21">
-        <v>44173.261400448537</v>
-      </c>
-    </row>
-    <row r="1250" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1250" spans="1:35" s="21" customFormat="1">
       <c r="A1250" s="19" t="s">
         <v>180</v>
       </c>
@@ -53187,11 +53142,8 @@
       <c r="AI1250" s="21">
         <v>16.329999999999998</v>
       </c>
-      <c r="AJ1250" s="21">
-        <v>57159.614147909968</v>
-      </c>
-    </row>
-    <row r="1251" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1251" spans="1:35" s="21" customFormat="1">
       <c r="A1251" s="19" t="s">
         <v>180</v>
       </c>
@@ -53246,11 +53198,8 @@
       <c r="AI1251" s="21">
         <v>22.95</v>
       </c>
-      <c r="AJ1251" s="21">
-        <v>50439.036772394567</v>
-      </c>
-    </row>
-    <row r="1252" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1252" spans="1:35" s="21" customFormat="1">
       <c r="A1252" s="19" t="s">
         <v>180</v>
       </c>
@@ -53305,11 +53254,8 @@
       <c r="AI1252" s="21">
         <v>27.3</v>
       </c>
-      <c r="AJ1252" s="21">
-        <v>48707.942128075207</v>
-      </c>
-    </row>
-    <row r="1253" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1253" spans="1:35" s="21" customFormat="1">
       <c r="A1253" s="19" t="s">
         <v>180</v>
       </c>
@@ -53323,7 +53269,7 @@
         <v>187.92</v>
       </c>
     </row>
-    <row r="1254" spans="1:36" s="21" customFormat="1">
+    <row r="1254" spans="1:35" s="21" customFormat="1">
       <c r="A1254" s="19" t="s">
         <v>180</v>
       </c>
@@ -53337,7 +53283,7 @@
         <v>219.89</v>
       </c>
     </row>
-    <row r="1255" spans="1:36" s="21" customFormat="1">
+    <row r="1255" spans="1:35" s="21" customFormat="1">
       <c r="A1255" s="19" t="s">
         <v>180</v>
       </c>
@@ -53351,7 +53297,7 @@
         <v>234.71</v>
       </c>
     </row>
-    <row r="1256" spans="1:36" s="21" customFormat="1">
+    <row r="1256" spans="1:35" s="21" customFormat="1">
       <c r="A1256" s="19" t="s">
         <v>180</v>
       </c>
@@ -53365,7 +53311,7 @@
         <v>241.95</v>
       </c>
     </row>
-    <row r="1257" spans="1:36" s="21" customFormat="1">
+    <row r="1257" spans="1:35" s="21" customFormat="1">
       <c r="A1257" s="19" t="s">
         <v>181</v>
       </c>
@@ -53420,11 +53366,8 @@
       <c r="AI1257" s="21">
         <v>1.1100000000000001</v>
       </c>
-      <c r="AJ1257" s="21">
-        <v>108933.67567567567</v>
-      </c>
-    </row>
-    <row r="1258" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1258" spans="1:35" s="21" customFormat="1">
       <c r="A1258" s="19" t="s">
         <v>181</v>
       </c>
@@ -53479,11 +53422,8 @@
       <c r="AI1258" s="21">
         <v>12.36</v>
       </c>
-      <c r="AJ1258" s="21">
-        <v>47236.548726243433</v>
-      </c>
-    </row>
-    <row r="1259" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1259" spans="1:35" s="21" customFormat="1">
       <c r="A1259" s="19" t="s">
         <v>181</v>
       </c>
@@ -53538,11 +53478,8 @@
       <c r="AI1259" s="21">
         <v>19.27</v>
       </c>
-      <c r="AJ1259" s="21">
-        <v>38374.057083549575</v>
-      </c>
-    </row>
-    <row r="1260" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1260" spans="1:35" s="21" customFormat="1">
       <c r="A1260" s="19" t="s">
         <v>181</v>
       </c>
@@ -53597,11 +53534,8 @@
       <c r="AI1260" s="21">
         <v>24.47</v>
       </c>
-      <c r="AJ1260" s="21">
-        <v>58212.351895371416</v>
-      </c>
-    </row>
-    <row r="1261" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1261" spans="1:35" s="21" customFormat="1">
       <c r="A1261" s="19" t="s">
         <v>181</v>
       </c>
@@ -53656,11 +53590,8 @@
       <c r="AI1261" s="21">
         <v>31.82</v>
       </c>
-      <c r="AJ1261" s="21">
-        <v>47291.42282554046</v>
-      </c>
-    </row>
-    <row r="1262" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1262" spans="1:35" s="21" customFormat="1">
       <c r="A1262" s="19" t="s">
         <v>181</v>
       </c>
@@ -53715,11 +53646,8 @@
       <c r="AI1262" s="21">
         <v>38.270000000000003</v>
       </c>
-      <c r="AJ1262" s="21">
-        <v>46127.351916376305</v>
-      </c>
-    </row>
-    <row r="1263" spans="1:36" s="21" customFormat="1">
+    </row>
+    <row r="1263" spans="1:35" s="21" customFormat="1">
       <c r="A1263" s="19" t="s">
         <v>181</v>
       </c>
@@ -53733,7 +53661,7 @@
         <v>246.74</v>
       </c>
     </row>
-    <row r="1264" spans="1:36" s="21" customFormat="1">
+    <row r="1264" spans="1:35" s="21" customFormat="1">
       <c r="A1264" s="19" t="s">
         <v>181</v>
       </c>

</xml_diff>

<commit_message>
Fixed Westfiled site stocking and copied DBH and Ht functions from globulus to nitens
</commit_message>
<xml_diff>
--- a/Tests/Validation/Eucalyptus/Observed.xlsx
+++ b/Tests/Validation/Eucalyptus/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Tests\Validation\Eucalyptus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144F369E-FB7A-4575-B639-C8D1D2E5DF0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380A22C7-79A9-42C5-A212-9597CC54F5A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="653" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18198,10 +18198,10 @@
   <dimension ref="A1:BV2656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5720" ySplit="1420" topLeftCell="N744" activePane="bottomRight"/>
+      <pane xSplit="5720" ySplit="1420" topLeftCell="C44" activePane="bottomRight"/>
       <selection pane="topRight" activeCell="BO1" sqref="BO1"/>
       <selection pane="bottomLeft" activeCell="A671" sqref="A671:E718"/>
-      <selection pane="bottomRight" activeCell="S719" sqref="S719:S758"/>
+      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="12.5"/>
@@ -18648,12 +18648,7 @@
       <c r="C8" s="28">
         <v>3.67</v>
       </c>
-      <c r="D8" s="28">
-        <v>95</v>
-      </c>
-      <c r="E8" s="21">
-        <v>1358.5</v>
-      </c>
+      <c r="D8" s="28"/>
       <c r="F8" s="21">
         <v>5524.9583865037248</v>
       </c>
@@ -18681,12 +18676,8 @@
       <c r="C9" s="28">
         <v>4.67</v>
       </c>
-      <c r="D9" s="28">
-        <v>94.166666666666671</v>
-      </c>
-      <c r="E9" s="28">
-        <v>1346.5833333333333</v>
-      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="21">
         <v>8246.2511632895439</v>
       </c>
@@ -18714,11 +18705,9 @@
       <c r="C10" s="28">
         <v>5.75</v>
       </c>
-      <c r="D10" s="28">
-        <v>93.333333333333329</v>
-      </c>
-      <c r="E10" s="28">
-        <v>1334.6666666666667</v>
+      <c r="D10" s="28"/>
+      <c r="E10" s="21">
+        <v>1430</v>
       </c>
       <c r="F10" s="21">
         <v>11405.035163989576</v>
@@ -18746,11 +18735,9 @@
       <c r="C11" s="28">
         <v>6.83</v>
       </c>
-      <c r="D11" s="28">
-        <v>92.5</v>
-      </c>
-      <c r="E11" s="28">
-        <v>1322.75</v>
+      <c r="D11" s="28"/>
+      <c r="E11" s="21">
+        <v>1418.0833333333335</v>
       </c>
       <c r="F11" s="21">
         <v>13895.85102605342</v>
@@ -18779,11 +18766,9 @@
       <c r="C12" s="28">
         <v>7.75</v>
       </c>
-      <c r="D12" s="28">
-        <v>77.585307781892809</v>
-      </c>
+      <c r="D12" s="28"/>
       <c r="E12" s="21">
-        <v>1109.8779999999999</v>
+        <v>1418.0833333333335</v>
       </c>
       <c r="F12" s="21">
         <v>15810.975455905455</v>
@@ -18843,6 +18828,9 @@
         <v>8.83</v>
       </c>
       <c r="D13" s="28"/>
+      <c r="E13" s="21">
+        <v>1418.0833333333335</v>
+      </c>
       <c r="F13" s="21">
         <v>17854.722043530433</v>
       </c>
@@ -18951,12 +18939,7 @@
       <c r="C17" s="28">
         <v>3.67</v>
       </c>
-      <c r="D17" s="28">
-        <v>95</v>
-      </c>
-      <c r="E17" s="21">
-        <v>1358.5</v>
-      </c>
+      <c r="D17" s="28"/>
       <c r="F17" s="21">
         <v>5212.444893285955</v>
       </c>
@@ -18984,12 +18967,8 @@
       <c r="C18" s="28">
         <v>4.67</v>
       </c>
-      <c r="D18" s="28">
-        <v>94.166666666666671</v>
-      </c>
-      <c r="E18" s="28">
-        <v>1346.5833333333333</v>
-      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
       <c r="F18" s="21">
         <v>7630.6674303207665</v>
       </c>
@@ -19017,11 +18996,9 @@
       <c r="C19" s="28">
         <v>5.75</v>
       </c>
-      <c r="D19" s="28">
-        <v>93.333333333333329</v>
-      </c>
+      <c r="D19" s="28"/>
       <c r="E19" s="28">
-        <v>1334.6666666666667</v>
+        <v>1358.5</v>
       </c>
       <c r="F19" s="21">
         <v>10003.546535546151</v>
@@ -19050,11 +19027,9 @@
       <c r="C20" s="28">
         <v>6.83</v>
       </c>
-      <c r="D20" s="28">
-        <v>93.333333333333329</v>
-      </c>
+      <c r="D20" s="28"/>
       <c r="E20" s="28">
-        <v>1334.6666666666667</v>
+        <v>1358.5</v>
       </c>
       <c r="F20" s="21">
         <v>11893.24907598501</v>
@@ -19083,11 +19058,9 @@
       <c r="C21" s="28">
         <v>7.75</v>
       </c>
-      <c r="D21" s="28">
-        <v>77.585307781892809</v>
-      </c>
+      <c r="D21" s="28"/>
       <c r="E21" s="21">
-        <v>1109.8779999999999</v>
+        <v>1358.5</v>
       </c>
       <c r="F21" s="21">
         <v>14014.328069578958</v>
@@ -19138,6 +19111,9 @@
         <v>8.83</v>
       </c>
       <c r="D22" s="28"/>
+      <c r="E22" s="21">
+        <v>1334.6666666666667</v>
+      </c>
       <c r="F22" s="21">
         <v>16080.422567432726</v>
       </c>
@@ -19218,12 +19194,7 @@
       <c r="C25" s="28">
         <v>2.75</v>
       </c>
-      <c r="D25" s="28">
-        <v>100</v>
-      </c>
-      <c r="E25" s="21">
-        <v>1430</v>
-      </c>
+      <c r="D25" s="28"/>
       <c r="F25" s="21">
         <v>2461.9500145108891</v>
       </c>
@@ -19251,12 +19222,7 @@
       <c r="C26" s="28">
         <v>3.67</v>
       </c>
-      <c r="D26" s="28">
-        <v>99.166666666666686</v>
-      </c>
-      <c r="E26" s="21">
-        <v>1418.0833333333335</v>
-      </c>
+      <c r="D26" s="28"/>
       <c r="F26" s="21">
         <v>6625.9230218877183</v>
       </c>
@@ -19284,12 +19250,7 @@
       <c r="C27" s="28">
         <v>4.67</v>
       </c>
-      <c r="D27" s="28">
-        <v>99.166666666666686</v>
-      </c>
-      <c r="E27" s="21">
-        <v>1418.0833333333335</v>
-      </c>
+      <c r="D27" s="28"/>
       <c r="F27" s="21">
         <v>9201.6754466831935</v>
       </c>
@@ -19317,11 +19278,9 @@
       <c r="C28" s="28">
         <v>5.75</v>
       </c>
-      <c r="D28" s="28">
-        <v>99.166666666666686</v>
-      </c>
+      <c r="D28" s="28"/>
       <c r="E28" s="21">
-        <v>1418.0833333333335</v>
+        <v>1382.3333333333333</v>
       </c>
       <c r="F28" s="21">
         <v>11873.361597578867</v>
@@ -19351,6 +19310,9 @@
         <v>6.83</v>
       </c>
       <c r="D29" s="28"/>
+      <c r="E29" s="21">
+        <v>1382.3333333333333</v>
+      </c>
       <c r="F29" s="21">
         <v>13585.618332417442</v>
       </c>
@@ -19378,11 +19340,9 @@
       <c r="C30" s="28">
         <v>7.75</v>
       </c>
-      <c r="D30" s="28">
-        <v>77.585307781892809</v>
-      </c>
+      <c r="D30" s="28"/>
       <c r="E30" s="21">
-        <v>1109.8779999999999</v>
+        <v>1382.3333333333333</v>
       </c>
       <c r="F30" s="21">
         <v>14983.847038686019</v>
@@ -19433,7 +19393,9 @@
         <v>8.83</v>
       </c>
       <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
+      <c r="E31" s="28">
+        <v>1382.3333333333333</v>
+      </c>
       <c r="F31" s="21">
         <v>16504.983712588109</v>
       </c>
@@ -19516,12 +19478,7 @@
       <c r="C34" s="28">
         <v>2.75</v>
       </c>
-      <c r="D34" s="28">
-        <v>95</v>
-      </c>
-      <c r="E34" s="21">
-        <v>1358.5</v>
-      </c>
+      <c r="D34" s="28"/>
       <c r="F34" s="21">
         <v>2816.6244066038712</v>
       </c>
@@ -19549,12 +19506,7 @@
       <c r="C35" s="28">
         <v>3.67</v>
       </c>
-      <c r="D35" s="28">
-        <v>95</v>
-      </c>
-      <c r="E35" s="21">
-        <v>1358.5</v>
-      </c>
+      <c r="D35" s="28"/>
       <c r="F35" s="21">
         <v>7425.9276045451097</v>
       </c>
@@ -19582,12 +19534,7 @@
       <c r="C36" s="28">
         <v>4.67</v>
       </c>
-      <c r="D36" s="28">
-        <v>95</v>
-      </c>
-      <c r="E36" s="21">
-        <v>1358.5</v>
-      </c>
+      <c r="D36" s="28"/>
       <c r="F36" s="21">
         <v>11005.887935097315</v>
       </c>
@@ -19615,11 +19562,9 @@
       <c r="C37" s="28">
         <v>5.75</v>
       </c>
-      <c r="D37" s="28">
-        <v>93.333333333333329</v>
-      </c>
+      <c r="D37" s="28"/>
       <c r="E37" s="21">
-        <v>1334.6666666666667</v>
+        <v>1406.1666666666665</v>
       </c>
       <c r="F37" s="21">
         <v>14618.667045628205</v>
@@ -19649,6 +19594,9 @@
         <v>6.83</v>
       </c>
       <c r="D38" s="28"/>
+      <c r="E38" s="21">
+        <v>1406.1666666666665</v>
+      </c>
       <c r="F38" s="21">
         <v>17066.403986702626</v>
       </c>
@@ -19676,11 +19624,9 @@
       <c r="C39" s="28">
         <v>7.75</v>
       </c>
-      <c r="D39" s="28">
-        <v>77.585307781892809</v>
-      </c>
+      <c r="D39" s="28"/>
       <c r="E39" s="21">
-        <v>1109.8779999999999</v>
+        <v>1406.1666666666665</v>
       </c>
       <c r="F39" s="21">
         <v>19153.612742048346</v>
@@ -19731,6 +19677,9 @@
         <v>8.83</v>
       </c>
       <c r="D40" s="28"/>
+      <c r="E40" s="21">
+        <v>1406.1666666666665</v>
+      </c>
       <c r="F40" s="21">
         <v>21050.282403902969</v>
       </c>
@@ -19811,12 +19760,8 @@
       <c r="C43" s="28">
         <v>2.75</v>
       </c>
-      <c r="D43" s="28">
-        <v>96.666666666666657</v>
-      </c>
-      <c r="E43" s="28">
-        <v>1382.3333333333333</v>
-      </c>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
       <c r="F43" s="21">
         <v>2576.5161955259723</v>
       </c>
@@ -19844,12 +19789,7 @@
       <c r="C44" s="28">
         <v>3.67</v>
       </c>
-      <c r="D44" s="28">
-        <v>96.666666666666657</v>
-      </c>
-      <c r="E44" s="21">
-        <v>1382.3333333333333</v>
-      </c>
+      <c r="D44" s="28"/>
       <c r="F44" s="21">
         <v>6928.0417055094249</v>
       </c>
@@ -19877,12 +19817,7 @@
       <c r="C45" s="28">
         <v>4.67</v>
       </c>
-      <c r="D45" s="28">
-        <v>96.666666666666657</v>
-      </c>
-      <c r="E45" s="21">
-        <v>1382.3333333333333</v>
-      </c>
+      <c r="D45" s="28"/>
       <c r="F45" s="21">
         <v>10175.281192318567</v>
       </c>
@@ -19910,11 +19845,9 @@
       <c r="C46" s="28">
         <v>5.75</v>
       </c>
-      <c r="D46" s="28">
-        <v>96.666666666666657</v>
-      </c>
+      <c r="D46" s="28"/>
       <c r="E46" s="21">
-        <v>1382.3333333333333</v>
+        <v>1358.5</v>
       </c>
       <c r="F46" s="21">
         <v>13800.203556211975</v>
@@ -19944,6 +19877,9 @@
         <v>6.83</v>
       </c>
       <c r="D47" s="28"/>
+      <c r="E47" s="21">
+        <v>1346.5833333333333</v>
+      </c>
       <c r="F47" s="21">
         <v>16083.126345739644</v>
       </c>
@@ -19971,11 +19907,9 @@
       <c r="C48" s="28">
         <v>7.75</v>
       </c>
-      <c r="D48" s="28">
-        <v>77.585307781892809</v>
-      </c>
+      <c r="D48" s="28"/>
       <c r="E48" s="21">
-        <v>1109.8779999999999</v>
+        <v>1334.6666666666667</v>
       </c>
       <c r="F48" s="21">
         <v>17830.838828209064</v>
@@ -20034,6 +19968,9 @@
         <v>8.83</v>
       </c>
       <c r="D49" s="28"/>
+      <c r="E49" s="21">
+        <v>1322.75</v>
+      </c>
       <c r="F49" s="21">
         <v>19478.992489987824</v>
       </c>
@@ -20114,12 +20051,7 @@
       <c r="C52" s="28">
         <v>2.75</v>
       </c>
-      <c r="D52" s="28">
-        <v>98.333333333333329</v>
-      </c>
-      <c r="E52" s="21">
-        <v>1406.1666666666665</v>
-      </c>
+      <c r="D52" s="28"/>
       <c r="F52" s="21">
         <v>2739.5403278341009</v>
       </c>
@@ -20147,12 +20079,7 @@
       <c r="C53" s="28">
         <v>3.67</v>
       </c>
-      <c r="D53" s="28">
-        <v>98.333333333333329</v>
-      </c>
-      <c r="E53" s="21">
-        <v>1406.1666666666665</v>
-      </c>
+      <c r="D53" s="28"/>
       <c r="F53" s="21">
         <v>6719.4405699830622</v>
       </c>
@@ -20180,12 +20107,7 @@
       <c r="C54" s="28">
         <v>4.67</v>
       </c>
-      <c r="D54" s="28">
-        <v>98.333333333333329</v>
-      </c>
-      <c r="E54" s="21">
-        <v>1406.1666666666665</v>
-      </c>
+      <c r="D54" s="28"/>
       <c r="F54" s="21">
         <v>9948.0058011851997</v>
       </c>
@@ -20213,11 +20135,9 @@
       <c r="C55" s="28">
         <v>5.75</v>
       </c>
-      <c r="D55" s="28">
-        <v>98.333333333333329</v>
-      </c>
+      <c r="D55" s="28"/>
       <c r="E55" s="21">
-        <v>1406.1666666666665</v>
+        <v>1358.5</v>
       </c>
       <c r="F55" s="21">
         <v>13379.955949576595</v>
@@ -20247,6 +20167,9 @@
         <v>6.83</v>
       </c>
       <c r="D56" s="28"/>
+      <c r="E56" s="21">
+        <v>1346.5833333333333</v>
+      </c>
       <c r="F56" s="21">
         <v>16192.485349000926</v>
       </c>
@@ -20274,11 +20197,9 @@
       <c r="C57" s="28">
         <v>7.75</v>
       </c>
-      <c r="D57" s="28">
-        <v>77.585307781892809</v>
-      </c>
+      <c r="D57" s="28"/>
       <c r="E57" s="21">
-        <v>1109.8779999999999</v>
+        <v>1334.6666666666667</v>
       </c>
       <c r="F57" s="21">
         <v>18356.171857481932</v>
@@ -20329,6 +20250,9 @@
         <v>8.83</v>
       </c>
       <c r="D58" s="28"/>
+      <c r="E58" s="21">
+        <v>1334.6666666666667</v>
+      </c>
       <c r="F58" s="21">
         <v>20310.18939754961</v>
       </c>
@@ -35352,10 +35276,10 @@
         <v>1.83</v>
       </c>
       <c r="D630" s="28">
-        <v>94.604992620810577</v>
+        <v>89.198993042478548</v>
       </c>
       <c r="E630" s="42">
-        <v>1050</v>
+        <v>990</v>
       </c>
       <c r="G630" s="29"/>
       <c r="AB630" s="21">
@@ -35376,10 +35300,10 @@
         <v>2.08</v>
       </c>
       <c r="D631" s="28">
-        <v>94.604992620810577</v>
+        <v>89.198993042478548</v>
       </c>
       <c r="E631" s="42">
-        <v>1050</v>
+        <v>990</v>
       </c>
       <c r="G631" s="29"/>
       <c r="AB631" s="21">
@@ -35901,10 +35825,10 @@
         <v>1.83</v>
       </c>
       <c r="D654" s="28">
-        <v>94.604992620810577</v>
+        <v>89.198993042478548</v>
       </c>
       <c r="E654" s="42">
-        <v>1050</v>
+        <v>990</v>
       </c>
       <c r="G654" s="29"/>
       <c r="AB654" s="21">
@@ -35925,10 +35849,10 @@
         <v>2.08</v>
       </c>
       <c r="D655" s="28">
-        <v>94.604992620810577</v>
+        <v>89.198993042478548</v>
       </c>
       <c r="E655" s="42">
-        <v>1050</v>
+        <v>990</v>
       </c>
       <c r="G655" s="29"/>
       <c r="AB655" s="21">
@@ -36450,10 +36374,10 @@
         <v>1.83</v>
       </c>
       <c r="D678" s="28">
-        <v>94.604992620810577</v>
+        <v>89.198993042478548</v>
       </c>
       <c r="E678" s="42">
-        <v>1050</v>
+        <v>990</v>
       </c>
       <c r="G678" s="29"/>
       <c r="AB678" s="21">
@@ -36474,10 +36398,10 @@
         <v>2.08</v>
       </c>
       <c r="D679" s="28">
-        <v>94.604992620810577</v>
+        <v>89.198993042478548</v>
       </c>
       <c r="E679" s="42">
-        <v>1050</v>
+        <v>990</v>
       </c>
       <c r="G679" s="29"/>
       <c r="AB679" s="21">
@@ -36991,7 +36915,7 @@
         <v>1.58</v>
       </c>
       <c r="D701" s="28">
-        <v>81.089993674980505</v>
+        <v>72.079994377760443</v>
       </c>
       <c r="E701" s="42">
         <v>900</v>
@@ -37413,9 +37337,7 @@
         <v>0.66</v>
       </c>
       <c r="D719" s="28"/>
-      <c r="E719" s="42">
-        <v>1109.8779999999999</v>
-      </c>
+      <c r="E719" s="42"/>
       <c r="F719" s="21">
         <v>609</v>
       </c>
@@ -37439,7 +37361,6 @@
         <v>366</v>
       </c>
       <c r="S719" s="21">
-        <f>M719/E719*10000</f>
         <v>1153.2799100441671</v>
       </c>
       <c r="W719" s="21">
@@ -37460,9 +37381,7 @@
         <v>1.04</v>
       </c>
       <c r="D720" s="28"/>
-      <c r="E720" s="42">
-        <v>900</v>
-      </c>
+      <c r="E720" s="42"/>
       <c r="F720" s="21">
         <v>1944.0000000000002</v>
       </c>
@@ -37486,7 +37405,6 @@
         <v>1479.0000000000002</v>
       </c>
       <c r="S720" s="21">
-        <f t="shared" ref="S720:S758" si="0">M720/E720*10000</f>
         <v>9111.1111111111113</v>
       </c>
       <c r="W720" s="21">
@@ -37507,9 +37425,7 @@
         <v>1.44</v>
       </c>
       <c r="D721" s="28"/>
-      <c r="E721" s="42">
-        <v>900</v>
-      </c>
+      <c r="E721" s="42"/>
       <c r="F721" s="21">
         <v>2437</v>
       </c>
@@ -37533,7 +37449,6 @@
         <v>1969</v>
       </c>
       <c r="S721" s="21">
-        <f t="shared" si="0"/>
         <v>13822.222222222223</v>
       </c>
       <c r="W721" s="21">
@@ -37554,9 +37469,7 @@
         <v>1.81</v>
       </c>
       <c r="D722" s="28"/>
-      <c r="E722" s="42">
-        <v>800</v>
-      </c>
+      <c r="E722" s="42"/>
       <c r="F722" s="21">
         <v>3062</v>
       </c>
@@ -37580,7 +37493,6 @@
         <v>2602</v>
       </c>
       <c r="S722" s="21">
-        <f t="shared" si="0"/>
         <v>23250</v>
       </c>
       <c r="W722" s="21">
@@ -37601,9 +37513,7 @@
         <v>2.4</v>
       </c>
       <c r="D723" s="28"/>
-      <c r="E723" s="42">
-        <v>800</v>
-      </c>
+      <c r="E723" s="42"/>
       <c r="F723" s="21">
         <v>3888.0000000000005</v>
       </c>
@@ -37627,7 +37537,6 @@
         <v>3492.0000000000005</v>
       </c>
       <c r="S723" s="21">
-        <f t="shared" si="0"/>
         <v>35937.5</v>
       </c>
       <c r="W723" s="21">
@@ -37648,9 +37557,7 @@
         <v>3.1</v>
       </c>
       <c r="D724" s="28"/>
-      <c r="E724" s="42">
-        <v>694</v>
-      </c>
+      <c r="E724" s="42"/>
       <c r="F724" s="21">
         <v>6311</v>
       </c>
@@ -37674,7 +37581,6 @@
         <v>5711</v>
       </c>
       <c r="S724" s="21">
-        <f t="shared" si="0"/>
         <v>67103.746397694529</v>
       </c>
       <c r="W724" s="21">
@@ -37695,9 +37601,7 @@
         <v>3.6</v>
       </c>
       <c r="D725" s="28"/>
-      <c r="E725" s="42">
-        <v>694</v>
-      </c>
+      <c r="E725" s="42"/>
       <c r="F725" s="21">
         <v>7158</v>
       </c>
@@ -37721,7 +37625,6 @@
         <v>6527</v>
       </c>
       <c r="S725" s="21">
-        <f t="shared" si="0"/>
         <v>76743.515850144089</v>
       </c>
       <c r="W725" s="21">
@@ -37742,9 +37645,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D726" s="28"/>
-      <c r="E726" s="42">
-        <v>694</v>
-      </c>
+      <c r="E726" s="42"/>
       <c r="F726" s="21">
         <v>8083</v>
       </c>
@@ -37768,7 +37669,6 @@
         <v>7418</v>
       </c>
       <c r="S726" s="21">
-        <f t="shared" si="0"/>
         <v>86657.060518731989</v>
       </c>
       <c r="W726" s="21">
@@ -37789,9 +37689,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D727" s="28"/>
-      <c r="E727" s="42">
-        <v>694</v>
-      </c>
+      <c r="E727" s="42"/>
       <c r="F727" s="21">
         <v>9853</v>
       </c>
@@ -37815,7 +37713,6 @@
         <v>9096</v>
       </c>
       <c r="S727" s="21">
-        <f t="shared" si="0"/>
         <v>105706.05187319883</v>
       </c>
       <c r="W727" s="21">
@@ -37836,9 +37733,7 @@
         <v>5.6</v>
       </c>
       <c r="D728" s="28"/>
-      <c r="E728" s="42">
-        <v>694</v>
-      </c>
+      <c r="E728" s="42"/>
       <c r="F728" s="21">
         <v>13702.000000000002</v>
       </c>
@@ -37862,7 +37757,6 @@
         <v>12765.000000000002</v>
       </c>
       <c r="S728" s="21">
-        <f t="shared" si="0"/>
         <v>146959.65417867436</v>
       </c>
       <c r="W728" s="21">
@@ -37883,9 +37777,7 @@
         <v>0.66</v>
       </c>
       <c r="D729" s="28"/>
-      <c r="E729" s="42">
-        <v>1050</v>
-      </c>
+      <c r="E729" s="42"/>
       <c r="F729" s="21">
         <v>36</v>
       </c>
@@ -37909,7 +37801,6 @@
         <v>17</v>
       </c>
       <c r="S729" s="21">
-        <f t="shared" si="0"/>
         <v>66.666666666666671</v>
       </c>
       <c r="W729" s="21">
@@ -37930,9 +37821,7 @@
         <v>1.04</v>
       </c>
       <c r="D730" s="28"/>
-      <c r="E730" s="42">
-        <v>1050</v>
-      </c>
+      <c r="E730" s="42"/>
       <c r="F730" s="21">
         <v>438.99999999999994</v>
       </c>
@@ -37956,7 +37845,6 @@
         <v>260.99999999999994</v>
       </c>
       <c r="S730" s="21">
-        <f t="shared" si="0"/>
         <v>885.71428571428567</v>
       </c>
       <c r="W730" s="21">
@@ -37977,9 +37865,7 @@
         <v>1.44</v>
       </c>
       <c r="D731" s="28"/>
-      <c r="E731" s="42">
-        <v>990</v>
-      </c>
+      <c r="E731" s="42"/>
       <c r="F731" s="21">
         <v>438.99999999999994</v>
       </c>
@@ -38003,7 +37889,6 @@
         <v>296.99999999999994</v>
       </c>
       <c r="S731" s="21">
-        <f t="shared" si="0"/>
         <v>1585.8585858585859</v>
       </c>
       <c r="W731" s="21">
@@ -38024,9 +37909,7 @@
         <v>1.81</v>
       </c>
       <c r="D732" s="28"/>
-      <c r="E732" s="42">
-        <v>990</v>
-      </c>
+      <c r="E732" s="42"/>
       <c r="F732" s="21">
         <v>501</v>
       </c>
@@ -38050,7 +37933,6 @@
         <v>401</v>
       </c>
       <c r="S732" s="21">
-        <f t="shared" si="0"/>
         <v>3141.4141414141418</v>
       </c>
       <c r="W732" s="21">
@@ -38071,9 +37953,7 @@
         <v>2.4</v>
       </c>
       <c r="D733" s="28"/>
-      <c r="E733" s="42">
-        <v>972</v>
-      </c>
+      <c r="E733" s="42"/>
       <c r="F733" s="21">
         <v>713</v>
       </c>
@@ -38097,7 +37977,6 @@
         <v>598</v>
       </c>
       <c r="S733" s="21">
-        <f t="shared" si="0"/>
         <v>5051.4403292181069</v>
       </c>
       <c r="W733" s="21">
@@ -38118,9 +37997,7 @@
         <v>3.1</v>
       </c>
       <c r="D734" s="28"/>
-      <c r="E734" s="42">
-        <v>694</v>
-      </c>
+      <c r="E734" s="42"/>
       <c r="F734" s="21">
         <v>1257</v>
       </c>
@@ -38144,7 +38021,6 @@
         <v>1123</v>
       </c>
       <c r="S734" s="21">
-        <f t="shared" si="0"/>
         <v>14077.809798270893</v>
       </c>
       <c r="W734" s="21">
@@ -38165,9 +38041,7 @@
         <v>3.6</v>
       </c>
       <c r="D735" s="28"/>
-      <c r="E735" s="42">
-        <v>694</v>
-      </c>
+      <c r="E735" s="42"/>
       <c r="F735" s="21">
         <v>1544</v>
       </c>
@@ -38190,7 +38064,6 @@
         <v>1392</v>
       </c>
       <c r="S735" s="21">
-        <f t="shared" si="0"/>
         <v>16945.244956772334</v>
       </c>
       <c r="W735" s="21">
@@ -38211,9 +38084,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D736" s="28"/>
-      <c r="E736" s="42">
-        <v>694</v>
-      </c>
+      <c r="E736" s="42"/>
       <c r="F736" s="21">
         <v>1960.0000000000002</v>
       </c>
@@ -38236,7 +38107,6 @@
         <v>1780.0000000000002</v>
       </c>
       <c r="S736" s="21">
-        <f t="shared" si="0"/>
         <v>21123.919308357348</v>
       </c>
       <c r="W736" s="21">
@@ -38257,9 +38127,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D737" s="28"/>
-      <c r="E737" s="42">
-        <v>694</v>
-      </c>
+      <c r="E737" s="42"/>
       <c r="F737" s="21">
         <v>2785</v>
       </c>
@@ -38282,7 +38150,6 @@
         <v>2546</v>
       </c>
       <c r="S737" s="21">
-        <f t="shared" si="0"/>
         <v>29495.677233429396</v>
       </c>
       <c r="W737" s="21">
@@ -38303,9 +38170,7 @@
         <v>5.6</v>
       </c>
       <c r="D738" s="28"/>
-      <c r="E738" s="42">
-        <v>694</v>
-      </c>
+      <c r="E738" s="42"/>
       <c r="F738" s="21">
         <v>4184</v>
       </c>
@@ -38328,7 +38193,6 @@
         <v>3862</v>
       </c>
       <c r="S738" s="21">
-        <f t="shared" si="0"/>
         <v>43587.89625360231</v>
       </c>
       <c r="W738" s="21">
@@ -38349,9 +38213,7 @@
         <v>0.66</v>
       </c>
       <c r="D739" s="28"/>
-      <c r="E739" s="42">
-        <v>1050</v>
-      </c>
+      <c r="E739" s="42"/>
       <c r="F739" s="21">
         <v>508</v>
       </c>
@@ -38374,7 +38236,6 @@
         <v>301</v>
       </c>
       <c r="S739" s="21">
-        <f t="shared" si="0"/>
         <v>1019.047619047619</v>
       </c>
       <c r="W739" s="21">
@@ -38395,9 +38256,7 @@
         <v>1.04</v>
       </c>
       <c r="D740" s="28"/>
-      <c r="E740" s="42">
-        <v>1050</v>
-      </c>
+      <c r="E740" s="42"/>
       <c r="F740" s="21">
         <v>1687</v>
       </c>
@@ -38420,7 +38279,6 @@
         <v>1262</v>
       </c>
       <c r="S740" s="21">
-        <f t="shared" si="0"/>
         <v>6466.6666666666661</v>
       </c>
       <c r="W740" s="21">
@@ -38441,9 +38299,7 @@
         <v>1.44</v>
       </c>
       <c r="D741" s="28"/>
-      <c r="E741" s="42">
-        <v>990</v>
-      </c>
+      <c r="E741" s="42"/>
       <c r="F741" s="21">
         <v>2581</v>
       </c>
@@ -38466,7 +38322,6 @@
         <v>2089</v>
       </c>
       <c r="S741" s="21">
-        <f t="shared" si="0"/>
         <v>13727.272727272728</v>
       </c>
       <c r="W741" s="21">
@@ -38487,9 +38342,7 @@
         <v>1.81</v>
       </c>
       <c r="D742" s="28"/>
-      <c r="E742" s="42">
-        <v>990</v>
-      </c>
+      <c r="E742" s="42"/>
       <c r="F742" s="21">
         <v>3347</v>
       </c>
@@ -38512,7 +38365,6 @@
         <v>2891</v>
       </c>
       <c r="S742" s="21">
-        <f t="shared" si="0"/>
         <v>22707.070707070707</v>
       </c>
       <c r="W742" s="21">
@@ -38533,9 +38385,7 @@
         <v>2.4</v>
       </c>
       <c r="D743" s="28"/>
-      <c r="E743" s="42">
-        <v>972</v>
-      </c>
+      <c r="E743" s="42"/>
       <c r="F743" s="21">
         <v>4990</v>
       </c>
@@ -38558,7 +38408,6 @@
         <v>4474</v>
       </c>
       <c r="S743" s="21">
-        <f t="shared" si="0"/>
         <v>38179.01234567901</v>
       </c>
       <c r="W743" s="21">
@@ -38579,9 +38428,7 @@
         <v>3.1</v>
       </c>
       <c r="D744" s="28"/>
-      <c r="E744" s="42">
-        <v>694</v>
-      </c>
+      <c r="E744" s="42"/>
       <c r="F744" s="21">
         <v>7203</v>
       </c>
@@ -38604,7 +38451,6 @@
         <v>6493</v>
       </c>
       <c r="S744" s="21">
-        <f t="shared" si="0"/>
         <v>75936.599423631123</v>
       </c>
       <c r="W744" s="21">
@@ -38625,9 +38471,7 @@
         <v>3.6</v>
       </c>
       <c r="D745" s="28"/>
-      <c r="E745" s="42">
-        <v>694</v>
-      </c>
+      <c r="E745" s="42"/>
       <c r="F745" s="21">
         <v>8305</v>
       </c>
@@ -38650,7 +38494,6 @@
         <v>7548</v>
       </c>
       <c r="S745" s="21">
-        <f t="shared" si="0"/>
         <v>87723.34293948127</v>
       </c>
       <c r="W745" s="21">
@@ -38671,9 +38514,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D746" s="28"/>
-      <c r="E746" s="42">
-        <v>694</v>
-      </c>
+      <c r="E746" s="42"/>
       <c r="F746" s="21">
         <v>9295</v>
       </c>
@@ -38696,7 +38537,6 @@
         <v>8504</v>
       </c>
       <c r="S746" s="21">
-        <f t="shared" si="0"/>
         <v>98242.074927953901</v>
       </c>
       <c r="W746" s="21">
@@ -38717,9 +38557,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D747" s="28"/>
-      <c r="E747" s="42">
-        <v>694</v>
-      </c>
+      <c r="E747" s="42"/>
       <c r="F747" s="21">
         <v>10620</v>
       </c>
@@ -38742,7 +38580,6 @@
         <v>9769</v>
       </c>
       <c r="S747" s="21">
-        <f t="shared" si="0"/>
         <v>112853.02593659944</v>
       </c>
       <c r="W747" s="21">
@@ -38763,9 +38600,7 @@
         <v>5.6</v>
       </c>
       <c r="D748" s="28"/>
-      <c r="E748" s="42">
-        <v>694</v>
-      </c>
+      <c r="E748" s="42"/>
       <c r="F748" s="21">
         <v>13559</v>
       </c>
@@ -38788,7 +38623,6 @@
         <v>12589</v>
       </c>
       <c r="S748" s="21">
-        <f t="shared" si="0"/>
         <v>143083.57348703171</v>
       </c>
       <c r="W748" s="21">
@@ -38809,9 +38643,7 @@
         <v>0.66</v>
       </c>
       <c r="D749" s="28"/>
-      <c r="E749" s="42">
-        <v>1050</v>
-      </c>
+      <c r="E749" s="42"/>
       <c r="F749" s="21">
         <v>17</v>
       </c>
@@ -38834,7 +38666,6 @@
         <v>8</v>
       </c>
       <c r="S749" s="21">
-        <f t="shared" si="0"/>
         <v>38.095238095238095</v>
       </c>
       <c r="W749" s="21">
@@ -38855,9 +38686,7 @@
         <v>1.04</v>
       </c>
       <c r="D750" s="28"/>
-      <c r="E750" s="42">
-        <v>1050</v>
-      </c>
+      <c r="E750" s="42"/>
       <c r="F750" s="21">
         <v>208</v>
       </c>
@@ -38880,7 +38709,6 @@
         <v>119</v>
       </c>
       <c r="S750" s="21">
-        <f t="shared" si="0"/>
         <v>428.57142857142856</v>
       </c>
       <c r="W750" s="21">
@@ -38901,9 +38729,7 @@
         <v>1.44</v>
       </c>
       <c r="D751" s="28"/>
-      <c r="E751" s="42">
-        <v>990</v>
-      </c>
+      <c r="E751" s="42"/>
       <c r="F751" s="21">
         <v>271</v>
       </c>
@@ -38926,7 +38752,6 @@
         <v>172</v>
       </c>
       <c r="S751" s="21">
-        <f t="shared" si="0"/>
         <v>808.0808080808082</v>
       </c>
       <c r="W751" s="21">
@@ -38947,9 +38772,7 @@
         <v>1.81</v>
       </c>
       <c r="D752" s="28"/>
-      <c r="E752" s="42">
-        <v>990</v>
-      </c>
+      <c r="E752" s="42"/>
       <c r="F752" s="21">
         <v>432</v>
       </c>
@@ -38972,7 +38795,6 @@
         <v>330</v>
       </c>
       <c r="S752" s="21">
-        <f t="shared" si="0"/>
         <v>2313.1313131313132</v>
       </c>
       <c r="W752" s="21">
@@ -38993,9 +38815,7 @@
         <v>2.4</v>
       </c>
       <c r="D753" s="28"/>
-      <c r="E753" s="42">
-        <v>972</v>
-      </c>
+      <c r="E753" s="42"/>
       <c r="F753" s="21">
         <v>818</v>
       </c>
@@ -39018,7 +38838,6 @@
         <v>666</v>
       </c>
       <c r="S753" s="21">
-        <f t="shared" si="0"/>
         <v>5061.7283950617284</v>
       </c>
       <c r="W753" s="21">
@@ -39039,9 +38858,7 @@
         <v>3.1</v>
       </c>
       <c r="D754" s="28"/>
-      <c r="E754" s="42">
-        <v>694</v>
-      </c>
+      <c r="E754" s="42"/>
       <c r="F754" s="21">
         <v>1443</v>
       </c>
@@ -39064,7 +38881,6 @@
         <v>1294</v>
       </c>
       <c r="S754" s="21">
-        <f t="shared" si="0"/>
         <v>16123.919308357348</v>
       </c>
       <c r="W754" s="21">
@@ -39085,9 +38901,7 @@
         <v>3.6</v>
       </c>
       <c r="D755" s="28"/>
-      <c r="E755" s="42">
-        <v>694</v>
-      </c>
+      <c r="E755" s="42"/>
       <c r="F755" s="21">
         <v>1847</v>
       </c>
@@ -39110,7 +38924,6 @@
         <v>1670</v>
       </c>
       <c r="S755" s="21">
-        <f t="shared" si="0"/>
         <v>20230.547550432275</v>
       </c>
       <c r="W755" s="21">
@@ -39131,9 +38944,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D756" s="28"/>
-      <c r="E756" s="42">
-        <v>694</v>
-      </c>
+      <c r="E756" s="42"/>
       <c r="F756" s="21">
         <v>2287</v>
       </c>
@@ -39156,7 +38967,6 @@
         <v>2083</v>
       </c>
       <c r="S756" s="21">
-        <f t="shared" si="0"/>
         <v>24726.224783861671</v>
       </c>
       <c r="W756" s="21">
@@ -39177,9 +38987,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D757" s="28"/>
-      <c r="E757" s="42">
-        <v>694</v>
-      </c>
+      <c r="E757" s="42"/>
       <c r="F757" s="21">
         <v>3025</v>
       </c>
@@ -39202,7 +39010,6 @@
         <v>2772</v>
       </c>
       <c r="S757" s="21">
-        <f t="shared" si="0"/>
         <v>32276.657060518733</v>
       </c>
       <c r="W757" s="21">
@@ -39223,9 +39030,7 @@
         <v>5.6</v>
       </c>
       <c r="D758" s="28"/>
-      <c r="E758" s="42">
-        <v>694</v>
-      </c>
+      <c r="E758" s="42"/>
       <c r="F758" s="21">
         <v>4188</v>
       </c>
@@ -39248,7 +39053,6 @@
         <v>3874</v>
       </c>
       <c r="S758" s="21">
-        <f t="shared" si="0"/>
         <v>44077.809798270893</v>
       </c>
       <c r="W758" s="21">
@@ -52352,7 +52156,7 @@
         <v>1453.0917380947396</v>
       </c>
       <c r="S1230" s="21">
-        <f t="shared" ref="S1230:S1234" si="1">M1230/E1230*10000</f>
+        <f t="shared" ref="S1230:S1234" si="0">M1230/E1230*10000</f>
         <v>11718.481758828546</v>
       </c>
       <c r="U1230" s="21">
@@ -52416,7 +52220,7 @@
         <v>3784.833849917014</v>
       </c>
       <c r="S1231" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30871.401712210554</v>
       </c>
       <c r="U1231" s="21">
@@ -52480,7 +52284,7 @@
         <v>7062.4584022535973</v>
       </c>
       <c r="S1232" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>58223.07009277492</v>
       </c>
       <c r="V1232" s="43">
@@ -52541,7 +52345,7 @@
         <v>9718.1440279723956</v>
       </c>
       <c r="S1233" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>82848.627689449248</v>
       </c>
       <c r="V1233" s="43">
@@ -52602,7 +52406,7 @@
         <v>11732.081554217362</v>
       </c>
       <c r="S1234" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>106076.68674699243</v>
       </c>
       <c r="U1234" s="21">
@@ -52740,7 +52544,7 @@
         <v>19847.535092434064</v>
       </c>
       <c r="S1239" s="21">
-        <f t="shared" ref="S1239" si="2">M1239/E1239*10000</f>
+        <f t="shared" ref="S1239" si="1">M1239/E1239*10000</f>
         <v>242931.88607630433</v>
       </c>
       <c r="U1239" s="21">
@@ -52865,7 +52669,7 @@
         <v>2317.7052375119029</v>
       </c>
       <c r="S1241" s="21">
-        <f t="shared" ref="S1241:S1245" si="3">M1241/E1241*10000</f>
+        <f t="shared" ref="S1241:S1245" si="2">M1241/E1241*10000</f>
         <v>9244.9351316789107</v>
       </c>
       <c r="U1241" s="21">
@@ -52929,7 +52733,7 @@
         <v>5292.0694450720694</v>
       </c>
       <c r="S1242" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>21804.98329242715</v>
       </c>
       <c r="U1242" s="21">
@@ -52993,7 +52797,7 @@
         <v>9844.1963569651525</v>
       </c>
       <c r="S1243" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>42912.800161138417</v>
       </c>
       <c r="V1243" s="43">
@@ -53054,7 +52858,7 @@
         <v>13145.510351194249</v>
       </c>
       <c r="S1244" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>60107.500462708042</v>
       </c>
       <c r="V1244" s="43">
@@ -53115,7 +52919,7 @@
         <v>16317.842044498891</v>
       </c>
       <c r="S1245" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>81589.210222494468</v>
       </c>
       <c r="V1245" s="43">
@@ -53255,7 +53059,7 @@
         <v>22619.608488073354</v>
       </c>
       <c r="S1250" s="21">
-        <f t="shared" ref="S1250" si="4">M1250/E1250*10000</f>
+        <f t="shared" ref="S1250" si="3">M1250/E1250*10000</f>
         <v>176302.48237001832</v>
       </c>
       <c r="V1250" s="43">
@@ -53379,7 +53183,7 @@
         <v>883.14685643901771</v>
       </c>
       <c r="S1252" s="21">
-        <f t="shared" ref="S1252:S1256" si="5">M1252/E1252*10000</f>
+        <f t="shared" ref="S1252:S1256" si="4">M1252/E1252*10000</f>
         <v>6762.2270783998292</v>
       </c>
       <c r="V1252" s="43">
@@ -53440,7 +53244,7 @@
         <v>2083.1945827940012</v>
       </c>
       <c r="S1253" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>15950.953926447175</v>
       </c>
       <c r="V1253" s="43">
@@ -53501,7 +53305,7 @@
         <v>4532.3365834993901</v>
       </c>
       <c r="S1254" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>35408.879558588982</v>
       </c>
       <c r="V1254" s="43">
@@ -53562,7 +53366,7 @@
         <v>6553.4680441862492</v>
       </c>
       <c r="S1255" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>52302.219027823223</v>
       </c>
       <c r="V1255" s="43">
@@ -53623,7 +53427,7 @@
         <v>9080.0180770464085</v>
       </c>
       <c r="S1256" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>75666.81730872007</v>
       </c>
       <c r="V1256" s="43">
@@ -53705,7 +53509,7 @@
         <v>10</v>
       </c>
       <c r="D1260" s="21">
-        <f t="shared" ref="D1260:D1261" si="6">E1260/E$1225*100</f>
+        <f t="shared" ref="D1260:D1261" si="5">E1260/E$1225*100</f>
         <v>86.196549137284322</v>
       </c>
       <c r="E1260" s="21">
@@ -53733,7 +53537,7 @@
         <v>12.1</v>
       </c>
       <c r="D1261" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>83.195798949737437</v>
       </c>
       <c r="E1261" s="21">
@@ -53758,7 +53562,7 @@
         <v>16038.983021426331</v>
       </c>
       <c r="S1261" s="21">
-        <f t="shared" ref="S1261" si="7">M1261/E1261*10000</f>
+        <f t="shared" ref="S1261" si="6">M1261/E1261*10000</f>
         <v>144625.63590104898</v>
       </c>
       <c r="V1261" s="43">
@@ -53877,7 +53681,7 @@
         <v>1320.0378834186677</v>
       </c>
       <c r="S1263" s="21">
-        <f t="shared" ref="S1263:S1267" si="8">M1263/E1263*10000</f>
+        <f t="shared" ref="S1263:S1267" si="7">M1263/E1263*10000</f>
         <v>5102.5816908336592</v>
       </c>
       <c r="V1263" s="43">
@@ -53938,7 +53742,7 @@
         <v>2668.5273415517941</v>
       </c>
       <c r="S1264" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>10315.14241032777</v>
       </c>
       <c r="V1264" s="43">
@@ -53999,7 +53803,7 @@
         <v>6693.037250926156</v>
       </c>
       <c r="S1265" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>26412.933113362888</v>
       </c>
       <c r="V1265" s="43">
@@ -54060,7 +53864,7 @@
         <v>8799.1791397126835</v>
       </c>
       <c r="S1266" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>35098.440924262795</v>
       </c>
       <c r="V1266" s="43">
@@ -54121,7 +53925,7 @@
         <v>12086.795940494598</v>
       </c>
       <c r="S1267" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>50361.649752060825</v>
       </c>
       <c r="V1267" s="43">
@@ -54203,7 +54007,7 @@
         <v>10</v>
       </c>
       <c r="D1271" s="21">
-        <f t="shared" ref="D1271:D1272" si="9">E1271/E$1226*100</f>
+        <f t="shared" ref="D1271:D1272" si="8">E1271/E$1226*100</f>
         <v>82.977127859017614</v>
       </c>
       <c r="E1271" s="21">
@@ -54231,7 +54035,7 @@
         <v>12.1</v>
       </c>
       <c r="D1272" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>76.565429321334832</v>
       </c>
       <c r="E1272" s="21">
@@ -54256,7 +54060,7 @@
         <v>20675.87223779206</v>
       </c>
       <c r="S1272" s="21">
-        <f t="shared" ref="S1272" si="10">M1272/E1272*10000</f>
+        <f t="shared" ref="S1272" si="9">M1272/E1272*10000</f>
         <v>101253.04719780637</v>
       </c>
       <c r="V1272" s="43">

</xml_diff>

<commit_message>
Worked on Ht, BA, Vo
</commit_message>
<xml_diff>
--- a/Tests/Validation/Eucalyptus/Observed.xlsx
+++ b/Tests/Validation/Eucalyptus/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Tests\Validation\Eucalyptus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E42446-0A1D-4E57-B26F-881FB8C3AA54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AAA965-C5E4-4180-92D2-A9116ECE848F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17670" tabRatio="653" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GympieBiomass" sheetId="1" r:id="rId1"/>
@@ -18198,10 +18198,10 @@
   <dimension ref="A1:BV2656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5715" ySplit="1425" topLeftCell="F1" activePane="bottomRight"/>
-      <selection pane="topRight" activeCell="BO1" sqref="BO1"/>
-      <selection pane="bottomLeft" activeCell="A671" sqref="A671:E718"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <pane xSplit="5715" ySplit="1425" topLeftCell="S42" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="AD1" sqref="AD1"/>
+      <selection pane="bottomLeft" activeCell="A271" sqref="A271"/>
+      <selection pane="bottomRight" activeCell="AD43" sqref="AD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -18733,6 +18733,10 @@
       <c r="AC10" s="21">
         <v>15.096934120374524</v>
       </c>
+      <c r="AE10" s="21">
+        <f t="shared" ref="AE10:AE13" si="1">(AC10/2)^2*3.14159*E10/10000</f>
+        <v>25.597825359506864</v>
+      </c>
       <c r="AF10" s="21">
         <v>139.40667447566162</v>
       </c>
@@ -18764,6 +18768,10 @@
       <c r="AC11" s="21">
         <v>16.509725318135974</v>
       </c>
+      <c r="AE11" s="21">
+        <f t="shared" si="1"/>
+        <v>30.357846645437739</v>
+      </c>
       <c r="AF11" s="21">
         <v>167.36501331721334</v>
       </c>
@@ -18825,6 +18833,10 @@
       <c r="AC12" s="21">
         <v>17.443425799782354</v>
       </c>
+      <c r="AE12" s="21">
+        <f t="shared" si="1"/>
+        <v>33.888693951392931</v>
+      </c>
       <c r="AF12" s="21">
         <v>188.96612069258379</v>
       </c>
@@ -18855,6 +18867,10 @@
       </c>
       <c r="AC13" s="21">
         <v>18.311062929457375</v>
+      </c>
+      <c r="AE13" s="21">
+        <f t="shared" si="1"/>
+        <v>37.343788756064804</v>
       </c>
       <c r="AF13" s="21">
         <v>248.97227764592799</v>
@@ -19025,6 +19041,10 @@
       <c r="AC19" s="21">
         <v>14.556162118903666</v>
       </c>
+      <c r="AE19" s="21">
+        <f t="shared" ref="AE19:AE22" si="2">(AC19/2)^2*3.14159*E19/10000</f>
+        <v>22.606999518410785</v>
+      </c>
       <c r="AF19" s="21">
         <v>133.06600086229204</v>
       </c>
@@ -19056,6 +19076,10 @@
       <c r="AC20" s="21">
         <v>15.638772707027496</v>
       </c>
+      <c r="AE20" s="21">
+        <f t="shared" si="2"/>
+        <v>26.094831246816685</v>
+      </c>
       <c r="AF20" s="21">
         <v>156.14235211034324</v>
       </c>
@@ -19108,6 +19132,10 @@
       <c r="AC21" s="21">
         <v>16.710648581455018</v>
       </c>
+      <c r="AE21" s="21">
+        <f t="shared" si="2"/>
+        <v>29.794477233631902</v>
+      </c>
       <c r="AF21" s="21">
         <v>181.34308150337998</v>
       </c>
@@ -19139,6 +19167,10 @@
       <c r="AC22" s="21">
         <v>17.813362946552196</v>
       </c>
+      <c r="AE22" s="21">
+        <f t="shared" si="2"/>
+        <v>33.262444435291087</v>
+      </c>
       <c r="AF22" s="21">
         <v>231.87330532112117</v>
       </c>
@@ -19307,6 +19339,10 @@
       <c r="AC28" s="21">
         <v>15.799840697795641</v>
       </c>
+      <c r="AE28" s="21">
+        <f t="shared" ref="AE28:AE31" si="3">(AC28/2)^2*3.14159*E28/10000</f>
+        <v>27.102397559309413</v>
+      </c>
       <c r="AF28" s="21">
         <v>152.14512203795954</v>
       </c>
@@ -19338,6 +19374,10 @@
       <c r="AC29" s="21">
         <v>16.682044554674004</v>
       </c>
+      <c r="AE29" s="21">
+        <f t="shared" si="3"/>
+        <v>30.21348684446761</v>
+      </c>
       <c r="AF29" s="21">
         <v>172.45436399035779</v>
       </c>
@@ -19390,6 +19430,10 @@
       <c r="AC30" s="21">
         <v>17.389385727672199</v>
       </c>
+      <c r="AE30" s="21">
+        <f t="shared" si="3"/>
+        <v>32.829992023043076</v>
+      </c>
       <c r="AF30" s="21">
         <v>189.88003773962174</v>
       </c>
@@ -19420,6 +19464,10 @@
       </c>
       <c r="AC31" s="21">
         <v>18.073908139830067</v>
+      </c>
+      <c r="AE31" s="21">
+        <f t="shared" si="3"/>
+        <v>35.465528540624199</v>
       </c>
       <c r="AF31" s="21">
         <v>255.56229942687821</v>
@@ -19591,6 +19639,10 @@
       <c r="AC37" s="21">
         <v>17.299435715182405</v>
       </c>
+      <c r="AE37" s="21">
+        <f t="shared" ref="AE37:AE40" si="4">(AC37/2)^2*3.14159*E37/10000</f>
+        <v>33.051424929693333</v>
+      </c>
       <c r="AF37" s="21">
         <v>178.67833141737816</v>
       </c>
@@ -19622,6 +19674,10 @@
       <c r="AC38" s="21">
         <v>18.461590681769689</v>
       </c>
+      <c r="AE38" s="21">
+        <f t="shared" si="4"/>
+        <v>37.641294358499749</v>
+      </c>
       <c r="AF38" s="21">
         <v>206.74798515350881</v>
       </c>
@@ -19674,6 +19730,10 @@
       <c r="AC39" s="21">
         <v>19.356684438140658</v>
       </c>
+      <c r="AE39" s="21">
+        <f t="shared" si="4"/>
+        <v>41.379787239167626</v>
+      </c>
       <c r="AF39" s="21">
         <v>230.55640351483257</v>
       </c>
@@ -19704,6 +19764,10 @@
       </c>
       <c r="AC40" s="21">
         <v>20.124669089803589</v>
+      </c>
+      <c r="AE40" s="21">
+        <f t="shared" si="4"/>
+        <v>44.72844594735448</v>
       </c>
       <c r="AF40" s="21">
         <v>295.85786034175953</v>
@@ -19874,6 +19938,10 @@
       <c r="AC46" s="21">
         <v>17.023328553681235</v>
       </c>
+      <c r="AE46" s="21">
+        <f t="shared" ref="AE46:AE49" si="5">(AC46/2)^2*3.14159*E46/10000</f>
+        <v>30.919902777711187</v>
+      </c>
       <c r="AF46" s="21">
         <v>174.67622931527399</v>
       </c>
@@ -19905,6 +19973,10 @@
       <c r="AC47" s="21">
         <v>18.253356303356615</v>
       </c>
+      <c r="AE47" s="21">
+        <f t="shared" si="5"/>
+        <v>35.237753398669867</v>
+      </c>
       <c r="AF47" s="21">
         <v>202.43265843502064</v>
       </c>
@@ -19965,6 +20037,10 @@
       <c r="AC48" s="21">
         <v>19.104696190382281</v>
       </c>
+      <c r="AE48" s="21">
+        <f t="shared" si="5"/>
+        <v>38.259791605583956</v>
+      </c>
       <c r="AF48" s="21">
         <v>223.07697055604172</v>
       </c>
@@ -19996,6 +20072,10 @@
       <c r="AC49" s="21">
         <v>19.884966429748559</v>
       </c>
+      <c r="AE49" s="21">
+        <f t="shared" si="5"/>
+        <v>41.078730059765689</v>
+      </c>
       <c r="AF49" s="21">
         <v>285.36972760037713</v>
       </c>
@@ -20164,6 +20244,10 @@
       <c r="AC55" s="21">
         <v>16.846321915196516</v>
       </c>
+      <c r="AE55" s="21">
+        <f t="shared" ref="AE55:AE58" si="6">(AC55/2)^2*3.14159*E55/10000</f>
+        <v>30.280242434731619</v>
+      </c>
       <c r="AF55" s="21">
         <v>174.88425810987945</v>
       </c>
@@ -20195,6 +20279,10 @@
       <c r="AC56" s="21">
         <v>18.36049183127454</v>
       </c>
+      <c r="AE56" s="21">
+        <f t="shared" si="6"/>
+        <v>35.652613471507259</v>
+      </c>
       <c r="AF56" s="21">
         <v>209.78832425820914</v>
       </c>
@@ -20247,6 +20335,10 @@
       <c r="AC57" s="21">
         <v>19.416361867341777</v>
       </c>
+      <c r="AE57" s="21">
+        <f t="shared" si="6"/>
+        <v>39.518280863914207</v>
+      </c>
       <c r="AF57" s="21">
         <v>236.09137477941377</v>
       </c>
@@ -20277,6 +20369,10 @@
       </c>
       <c r="AC58" s="21">
         <v>20.221372277641578</v>
+      </c>
+      <c r="AE58" s="21">
+        <f t="shared" si="6"/>
+        <v>42.86310005042224</v>
       </c>
       <c r="AF58" s="21">
         <v>306.37150583325547</v>
@@ -27728,16 +27824,11 @@
       <c r="O331" s="42">
         <v>7600</v>
       </c>
-      <c r="P331" s="42">
-        <v>1000</v>
-      </c>
-      <c r="Q331" s="42">
-        <f>O331+P331</f>
-        <v>8600</v>
-      </c>
+      <c r="P331" s="42"/>
+      <c r="Q331" s="42"/>
       <c r="T331" s="21">
         <f>Q331/F331</f>
-        <v>0.34959349593495936</v>
+        <v>0</v>
       </c>
       <c r="W331" s="21">
         <v>5.8</v>
@@ -27889,16 +27980,11 @@
       <c r="O339" s="42">
         <v>2700</v>
       </c>
-      <c r="P339" s="42">
-        <v>3200</v>
-      </c>
-      <c r="Q339" s="42">
-        <f>O339+P339</f>
-        <v>5900</v>
-      </c>
+      <c r="P339" s="42"/>
+      <c r="Q339" s="42"/>
       <c r="T339" s="21">
         <f>Q339/F339</f>
-        <v>0.24380165289256198</v>
+        <v>0</v>
       </c>
       <c r="W339" s="21">
         <v>4.5</v>
@@ -50824,6 +50910,10 @@
       <c r="AC1184" s="21">
         <v>6</v>
       </c>
+      <c r="AE1184" s="21">
+        <f t="shared" ref="AE1184:AE1186" si="7">(AC1184/2)^2*3.14159*E1184/10000</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="1185" spans="1:67" s="21" customFormat="1">
       <c r="A1185" s="19" t="s">
@@ -50853,6 +50943,10 @@
       <c r="AC1185" s="21">
         <v>10.9</v>
       </c>
+      <c r="AE1185" s="21">
+        <f t="shared" si="7"/>
+        <v>13.390426545912499</v>
+      </c>
     </row>
     <row r="1186" spans="1:67" s="21" customFormat="1">
       <c r="A1186" s="19" t="s">
@@ -50882,6 +50976,10 @@
       <c r="AC1186" s="21">
         <v>12.6</v>
       </c>
+      <c r="AE1186" s="21">
+        <f t="shared" si="7"/>
+        <v>17.119896784830001</v>
+      </c>
     </row>
     <row r="1187" spans="1:67" s="21" customFormat="1">
       <c r="A1187" s="19" t="s">
@@ -50958,6 +51056,10 @@
       <c r="AC1188" s="21">
         <v>14.4</v>
       </c>
+      <c r="AE1188" s="21">
+        <f t="shared" ref="AE1188:AE1192" si="8">(AC1188/2)^2*3.14159*E1188/10000</f>
+        <v>21.85581543552</v>
+      </c>
     </row>
     <row r="1189" spans="1:67" s="21" customFormat="1">
       <c r="A1189" s="19" t="s">
@@ -50987,6 +51089,10 @@
       <c r="AC1189" s="21">
         <v>17.100000000000001</v>
       </c>
+      <c r="AE1189" s="21">
+        <f t="shared" si="8"/>
+        <v>30.820114735244999</v>
+      </c>
     </row>
     <row r="1190" spans="1:67" s="21" customFormat="1">
       <c r="A1190" s="19" t="s">
@@ -51016,6 +51122,10 @@
       <c r="AC1190" s="21">
         <v>17.899999999999999</v>
       </c>
+      <c r="AE1190" s="21">
+        <f t="shared" si="8"/>
+        <v>33.393850561782493</v>
+      </c>
     </row>
     <row r="1191" spans="1:67" s="21" customFormat="1">
       <c r="A1191" s="19" t="s">
@@ -51045,6 +51155,10 @@
       <c r="AC1191" s="21">
         <v>18.899999999999999</v>
       </c>
+      <c r="AE1191" s="21">
+        <f t="shared" si="8"/>
+        <v>37.229229297382496</v>
+      </c>
     </row>
     <row r="1192" spans="1:67" s="21" customFormat="1">
       <c r="A1192" s="19" t="s">
@@ -51074,6 +51188,10 @@
       <c r="AC1192" s="21">
         <v>19.5</v>
       </c>
+      <c r="AE1192" s="21">
+        <f t="shared" si="8"/>
+        <v>39.182538797999996</v>
+      </c>
     </row>
     <row r="1193" spans="1:67" s="21" customFormat="1">
       <c r="A1193" s="19" t="s">
@@ -51117,6 +51235,10 @@
       <c r="AC1194" s="21">
         <v>6.5</v>
       </c>
+      <c r="AE1194" s="21">
+        <f t="shared" ref="AE1194:AE1196" si="9">(AC1194/2)^2*3.14159*E1194/10000</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="1195" spans="1:67" s="21" customFormat="1">
       <c r="A1195" s="19" t="s">
@@ -51146,6 +51268,10 @@
       <c r="AC1195" s="21">
         <v>10.6</v>
       </c>
+      <c r="AE1195" s="21">
+        <f t="shared" si="9"/>
+        <v>15.390322684640001</v>
+      </c>
     </row>
     <row r="1196" spans="1:67" s="21" customFormat="1">
       <c r="A1196" s="19" t="s">
@@ -51175,6 +51301,10 @@
       <c r="AC1196" s="21">
         <v>12.2</v>
       </c>
+      <c r="AE1196" s="21">
+        <f t="shared" si="9"/>
+        <v>20.200071841919996</v>
+      </c>
     </row>
     <row r="1197" spans="1:67" s="21" customFormat="1">
       <c r="A1197" s="19" t="s">
@@ -51251,6 +51381,10 @@
       <c r="AC1198" s="21">
         <v>14.4</v>
       </c>
+      <c r="AE1198" s="21">
+        <f t="shared" ref="AE1198:AE1224" si="10">(AC1198/2)^2*3.14159*E1198/10000</f>
+        <v>28.14221242368</v>
+      </c>
     </row>
     <row r="1199" spans="1:67" s="21" customFormat="1">
       <c r="A1199" s="19" t="s">
@@ -51280,6 +51414,10 @@
       <c r="AC1199" s="21">
         <v>15.3</v>
       </c>
+      <c r="AE1199" s="21">
+        <f t="shared" si="10"/>
+        <v>31.494138942757505</v>
+      </c>
     </row>
     <row r="1200" spans="1:67" s="21" customFormat="1">
       <c r="A1200" s="19" t="s">
@@ -51309,6 +51447,10 @@
       <c r="AC1200" s="21">
         <v>16.100000000000001</v>
       </c>
+      <c r="AE1200" s="21">
+        <f t="shared" si="10"/>
+        <v>34.8737483675175</v>
+      </c>
     </row>
     <row r="1201" spans="1:67" s="21" customFormat="1">
       <c r="A1201" s="19" t="s">
@@ -51338,6 +51480,10 @@
       <c r="AC1201" s="21">
         <v>16.600000000000001</v>
       </c>
+      <c r="AE1201" s="21">
+        <f t="shared" si="10"/>
+        <v>36.402539523820003</v>
+      </c>
     </row>
     <row r="1202" spans="1:67" s="21" customFormat="1">
       <c r="A1202" s="19" t="s">
@@ -51395,6 +51541,10 @@
       <c r="AC1204" s="21">
         <v>6</v>
       </c>
+      <c r="AE1204" s="21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="1205" spans="1:67" s="21" customFormat="1">
       <c r="A1205" s="19" t="s">
@@ -51424,6 +51574,10 @@
       <c r="AC1205" s="21">
         <v>10.9</v>
       </c>
+      <c r="AE1205" s="21">
+        <f t="shared" si="10"/>
+        <v>13.390426545912499</v>
+      </c>
     </row>
     <row r="1206" spans="1:67" s="21" customFormat="1">
       <c r="A1206" s="19" t="s">
@@ -51453,6 +51607,10 @@
       <c r="AC1206" s="21">
         <v>12.6</v>
       </c>
+      <c r="AE1206" s="21">
+        <f t="shared" si="10"/>
+        <v>17.119896784830001</v>
+      </c>
     </row>
     <row r="1207" spans="1:67" s="21" customFormat="1">
       <c r="A1207" s="19" t="s">
@@ -51529,6 +51687,10 @@
       <c r="AC1208" s="21">
         <v>14.4</v>
       </c>
+      <c r="AE1208" s="21">
+        <f t="shared" si="10"/>
+        <v>21.85581543552</v>
+      </c>
     </row>
     <row r="1209" spans="1:67" s="21" customFormat="1">
       <c r="A1209" s="19" t="s">
@@ -51558,6 +51720,10 @@
       <c r="AC1209" s="21">
         <v>17.100000000000001</v>
       </c>
+      <c r="AE1209" s="21">
+        <f t="shared" si="10"/>
+        <v>30.820114735244999</v>
+      </c>
     </row>
     <row r="1210" spans="1:67" s="21" customFormat="1">
       <c r="A1210" s="19" t="s">
@@ -51587,6 +51753,10 @@
       <c r="AC1210" s="21">
         <v>17.899999999999999</v>
       </c>
+      <c r="AE1210" s="21">
+        <f t="shared" si="10"/>
+        <v>33.393850561782493</v>
+      </c>
     </row>
     <row r="1211" spans="1:67" s="21" customFormat="1">
       <c r="A1211" s="19" t="s">
@@ -51616,6 +51786,10 @@
       <c r="AC1211" s="21">
         <v>18.899999999999999</v>
       </c>
+      <c r="AE1211" s="21">
+        <f t="shared" si="10"/>
+        <v>37.229229297382496</v>
+      </c>
     </row>
     <row r="1212" spans="1:67" s="21" customFormat="1">
       <c r="A1212" s="19" t="s">
@@ -51645,6 +51819,10 @@
       <c r="AC1212" s="21">
         <v>19.5</v>
       </c>
+      <c r="AE1212" s="21">
+        <f t="shared" si="10"/>
+        <v>39.182538797999996</v>
+      </c>
     </row>
     <row r="1213" spans="1:67" s="21" customFormat="1">
       <c r="A1213" s="19" t="s">
@@ -51688,6 +51866,10 @@
       <c r="AC1214" s="21">
         <v>6.5</v>
       </c>
+      <c r="AE1214" s="21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="1215" spans="1:67" s="21" customFormat="1">
       <c r="A1215" s="19" t="s">
@@ -51717,6 +51899,10 @@
       <c r="AC1215" s="21">
         <v>10.6</v>
       </c>
+      <c r="AE1215" s="21">
+        <f t="shared" si="10"/>
+        <v>15.390322684640001</v>
+      </c>
     </row>
     <row r="1216" spans="1:67" s="21" customFormat="1">
       <c r="A1216" s="19" t="s">
@@ -51746,6 +51932,10 @@
       <c r="AC1216" s="21">
         <v>12.2</v>
       </c>
+      <c r="AE1216" s="21">
+        <f t="shared" si="10"/>
+        <v>20.200071841919996</v>
+      </c>
     </row>
     <row r="1217" spans="1:67" s="21" customFormat="1">
       <c r="A1217" s="19" t="s">
@@ -51822,6 +52012,10 @@
       <c r="AC1218" s="21">
         <v>14.4</v>
       </c>
+      <c r="AE1218" s="21">
+        <f t="shared" si="10"/>
+        <v>28.14221242368</v>
+      </c>
     </row>
     <row r="1219" spans="1:67" s="21" customFormat="1">
       <c r="A1219" s="19" t="s">
@@ -51851,6 +52045,10 @@
       <c r="AC1219" s="21">
         <v>15.3</v>
       </c>
+      <c r="AE1219" s="21">
+        <f t="shared" si="10"/>
+        <v>31.494138942757505</v>
+      </c>
     </row>
     <row r="1220" spans="1:67" s="21" customFormat="1">
       <c r="A1220" s="19" t="s">
@@ -51880,6 +52078,10 @@
       <c r="AC1220" s="21">
         <v>16.100000000000001</v>
       </c>
+      <c r="AE1220" s="21">
+        <f t="shared" si="10"/>
+        <v>34.8737483675175</v>
+      </c>
     </row>
     <row r="1221" spans="1:67" s="21" customFormat="1">
       <c r="A1221" s="19" t="s">
@@ -51909,6 +52111,10 @@
       <c r="AC1221" s="21">
         <v>16.600000000000001</v>
       </c>
+      <c r="AE1221" s="21">
+        <f t="shared" si="10"/>
+        <v>36.402539523820003</v>
+      </c>
     </row>
     <row r="1222" spans="1:67" s="21" customFormat="1">
       <c r="A1222" s="19" t="s">
@@ -51964,6 +52170,10 @@
       <c r="AC1223" s="21">
         <v>21.4</v>
       </c>
+      <c r="AE1223" s="21">
+        <f t="shared" si="10"/>
+        <v>31.903672688169994</v>
+      </c>
       <c r="BO1223" s="21">
         <v>20208</v>
       </c>
@@ -52008,6 +52218,10 @@
       <c r="AC1224" s="21">
         <v>18.399999999999999</v>
       </c>
+      <c r="AE1224" s="21">
+        <f t="shared" si="10"/>
+        <v>20.84688752384</v>
+      </c>
       <c r="BO1224" s="21">
         <v>5854.2</v>
       </c>
@@ -52120,6 +52334,10 @@
       <c r="AC1229" s="21">
         <v>2.88</v>
       </c>
+      <c r="AE1229" s="21">
+        <f t="shared" ref="AE1229" si="11">(AC1229/2)^2*3.14159*E1229/10000</f>
+        <v>0.79866556554239998</v>
+      </c>
       <c r="AF1229" s="21">
         <v>2.79</v>
       </c>
@@ -52168,7 +52386,7 @@
         <v>1453.0917380947396</v>
       </c>
       <c r="S1230" s="21">
-        <f t="shared" ref="S1230:S1234" si="1">M1230/E1230*10000</f>
+        <f t="shared" ref="S1230:S1234" si="12">M1230/E1230*10000</f>
         <v>11718.481758828546</v>
       </c>
       <c r="U1230" s="21">
@@ -52184,6 +52402,10 @@
       <c r="AC1230" s="21">
         <v>8.77</v>
       </c>
+      <c r="AE1230" s="21">
+        <f t="shared" ref="AE1230:AE1234" si="13">(AC1230/2)^2*3.14159*E1230/10000</f>
+        <v>7.4904927228409983</v>
+      </c>
       <c r="AF1230" s="21">
         <v>24.28</v>
       </c>
@@ -52232,7 +52454,7 @@
         <v>3784.833849917014</v>
       </c>
       <c r="S1231" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>30871.401712210554</v>
       </c>
       <c r="U1231" s="21">
@@ -52248,6 +52470,10 @@
       <c r="AC1231" s="21">
         <v>11.73</v>
       </c>
+      <c r="AE1231" s="21">
+        <f t="shared" si="13"/>
+        <v>13.24878367249215</v>
+      </c>
       <c r="AF1231" s="21">
         <v>66.95</v>
       </c>
@@ -52296,7 +52522,7 @@
         <v>7062.4584022535973</v>
       </c>
       <c r="S1232" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>58223.07009277492</v>
       </c>
       <c r="V1232" s="43">
@@ -52309,6 +52535,10 @@
       <c r="AC1232" s="21">
         <v>13.14</v>
       </c>
+      <c r="AE1232" s="21">
+        <f t="shared" si="13"/>
+        <v>16.449058526568301</v>
+      </c>
       <c r="AF1232" s="21">
         <v>110.06</v>
       </c>
@@ -52357,7 +52587,7 @@
         <v>9718.1440279723956</v>
       </c>
       <c r="S1233" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>82848.627689449248</v>
       </c>
       <c r="V1233" s="43">
@@ -52370,6 +52600,10 @@
       <c r="AC1233" s="21">
         <v>15.28</v>
       </c>
+      <c r="AE1233" s="21">
+        <f t="shared" si="13"/>
+        <v>21.509694150187197</v>
+      </c>
       <c r="AF1233" s="21">
         <v>153.4</v>
       </c>
@@ -52418,7 +52652,7 @@
         <v>11732.081554217362</v>
       </c>
       <c r="S1234" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>106076.68674699243</v>
       </c>
       <c r="U1234" s="21">
@@ -52434,6 +52668,10 @@
       <c r="AC1234" s="21">
         <v>16.63</v>
       </c>
+      <c r="AE1234" s="21">
+        <f t="shared" si="13"/>
+        <v>24.023105024173148</v>
+      </c>
       <c r="AF1234" s="21">
         <v>204.3</v>
       </c>
@@ -52556,7 +52794,7 @@
         <v>19847.535092434064</v>
       </c>
       <c r="S1239" s="21">
-        <f t="shared" ref="S1239" si="2">M1239/E1239*10000</f>
+        <f t="shared" ref="S1239" si="14">M1239/E1239*10000</f>
         <v>242931.88607630433</v>
       </c>
       <c r="U1239" s="21">
@@ -52633,6 +52871,10 @@
       <c r="AC1240" s="21">
         <v>2.5099999999999998</v>
       </c>
+      <c r="AE1240" s="21">
+        <f>(AC1240/2)^2*3.14159*E1240/10000</f>
+        <v>1.2271245318579997</v>
+      </c>
       <c r="AF1240" s="21">
         <v>3.46</v>
       </c>
@@ -52681,7 +52923,7 @@
         <v>2317.7052375119029</v>
       </c>
       <c r="S1241" s="21">
-        <f t="shared" ref="S1241:S1245" si="3">M1241/E1241*10000</f>
+        <f t="shared" ref="S1241:S1245" si="15">M1241/E1241*10000</f>
         <v>9244.9351316789107</v>
       </c>
       <c r="U1241" s="21">
@@ -52697,6 +52939,10 @@
       <c r="AC1241" s="21">
         <v>7.46</v>
       </c>
+      <c r="AE1241" s="21">
+        <f t="shared" ref="AE1241:AE1245" si="16">(AC1241/2)^2*3.14159*E1241/10000</f>
+        <v>10.957752917007701</v>
+      </c>
       <c r="AF1241" s="21">
         <v>38.54</v>
       </c>
@@ -52745,7 +52991,7 @@
         <v>5292.0694450720694</v>
       </c>
       <c r="S1242" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>21804.98329242715</v>
       </c>
       <c r="U1242" s="21">
@@ -52761,6 +53007,10 @@
       <c r="AC1242" s="21">
         <v>9.77</v>
       </c>
+      <c r="AE1242" s="21">
+        <f t="shared" si="16"/>
+        <v>18.194847433034923</v>
+      </c>
       <c r="AF1242" s="21">
         <v>99.7</v>
       </c>
@@ -52809,7 +53059,7 @@
         <v>9844.1963569651525</v>
       </c>
       <c r="S1243" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>42912.800161138417</v>
       </c>
       <c r="V1243" s="43">
@@ -52822,6 +53072,10 @@
       <c r="AC1243" s="21">
         <v>11.13</v>
       </c>
+      <c r="AE1243" s="21">
+        <f t="shared" si="16"/>
+        <v>22.31892417604185</v>
+      </c>
       <c r="AF1243" s="21">
         <v>141.69999999999999</v>
       </c>
@@ -52870,7 +53124,7 @@
         <v>13145.510351194249</v>
       </c>
       <c r="S1244" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>60107.500462708042</v>
       </c>
       <c r="V1244" s="43">
@@ -52883,6 +53137,10 @@
       <c r="AC1244" s="21">
         <v>12.39</v>
       </c>
+      <c r="AE1244" s="21">
+        <f t="shared" si="16"/>
+        <v>26.368225877717325</v>
+      </c>
       <c r="AF1244" s="21">
         <v>191.72</v>
       </c>
@@ -52931,7 +53189,7 @@
         <v>16317.842044498891</v>
       </c>
       <c r="S1245" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="15"/>
         <v>81589.210222494468</v>
       </c>
       <c r="V1245" s="43">
@@ -52943,6 +53201,10 @@
       <c r="Z1245" s="43"/>
       <c r="AC1245" s="21">
         <v>14.16</v>
+      </c>
+      <c r="AE1245" s="21">
+        <f t="shared" si="16"/>
+        <v>31.495319395199999</v>
       </c>
       <c r="AF1245" s="21">
         <v>233.71</v>
@@ -53071,7 +53333,7 @@
         <v>22619.608488073354</v>
       </c>
       <c r="S1250" s="21">
-        <f t="shared" ref="S1250" si="4">M1250/E1250*10000</f>
+        <f t="shared" ref="S1250" si="17">M1250/E1250*10000</f>
         <v>176302.48237001832</v>
       </c>
       <c r="V1250" s="43">
@@ -53147,6 +53409,10 @@
       <c r="AC1251" s="21">
         <v>1.39</v>
       </c>
+      <c r="AE1251" s="21">
+        <f>(AC1251/2)^2*3.14159*E1251/10000</f>
+        <v>0.19818112617334996</v>
+      </c>
       <c r="AF1251" s="21">
         <v>0.78</v>
       </c>
@@ -53195,7 +53461,7 @@
         <v>883.14685643901771</v>
       </c>
       <c r="S1252" s="21">
-        <f t="shared" ref="S1252:S1256" si="5">M1252/E1252*10000</f>
+        <f t="shared" ref="S1252:S1256" si="18">M1252/E1252*10000</f>
         <v>6762.2270783998292</v>
       </c>
       <c r="V1252" s="43">
@@ -53208,6 +53474,10 @@
       <c r="AC1252" s="21">
         <v>7.08</v>
       </c>
+      <c r="AE1252" s="21">
+        <f t="shared" ref="AE1252:AE1256" si="19">(AC1252/2)^2*3.14159*E1252/10000</f>
+        <v>5.1416108912664003</v>
+      </c>
       <c r="AF1252" s="21">
         <v>14.7</v>
       </c>
@@ -53256,7 +53526,7 @@
         <v>2083.1945827940012</v>
       </c>
       <c r="S1253" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>15950.953926447175</v>
       </c>
       <c r="V1253" s="43">
@@ -53269,6 +53539,10 @@
       <c r="AC1253" s="21">
         <v>10.02</v>
       </c>
+      <c r="AE1253" s="21">
+        <f t="shared" si="19"/>
+        <v>10.298361544565399</v>
+      </c>
       <c r="AF1253" s="21">
         <v>41.33</v>
       </c>
@@ -53317,7 +53591,7 @@
         <v>4532.3365834993901</v>
       </c>
       <c r="S1254" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>35408.879558588982</v>
       </c>
       <c r="V1254" s="43">
@@ -53330,6 +53604,10 @@
       <c r="AC1254" s="21">
         <v>11.73</v>
       </c>
+      <c r="AE1254" s="21">
+        <f t="shared" si="19"/>
+        <v>13.832335318752</v>
+      </c>
       <c r="AF1254" s="21">
         <v>76.42</v>
       </c>
@@ -53378,7 +53656,7 @@
         <v>6553.4680441862492</v>
       </c>
       <c r="S1255" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>52302.219027823223</v>
       </c>
       <c r="V1255" s="43">
@@ -53391,6 +53669,10 @@
       <c r="AC1255" s="21">
         <v>13.73</v>
       </c>
+      <c r="AE1255" s="21">
+        <f t="shared" si="19"/>
+        <v>18.551612315332076</v>
+      </c>
       <c r="AF1255" s="21">
         <v>118.19</v>
       </c>
@@ -53439,7 +53721,7 @@
         <v>9080.0180770464085</v>
       </c>
       <c r="S1256" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>75666.81730872007</v>
       </c>
       <c r="V1256" s="43">
@@ -53452,6 +53734,10 @@
       <c r="AC1256" s="21">
         <v>15.33</v>
       </c>
+      <c r="AE1256" s="21">
+        <f t="shared" si="19"/>
+        <v>22.149048304530002</v>
+      </c>
       <c r="AF1256" s="21">
         <v>162.19</v>
       </c>
@@ -53521,7 +53807,7 @@
         <v>10</v>
       </c>
       <c r="D1260" s="21">
-        <f t="shared" ref="D1260:D1261" si="6">E1260/E$1225*100</f>
+        <f t="shared" ref="D1260:D1261" si="20">E1260/E$1225*100</f>
         <v>86.196549137284322</v>
       </c>
       <c r="E1260" s="21">
@@ -53549,7 +53835,7 @@
         <v>12.1</v>
       </c>
       <c r="D1261" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="20"/>
         <v>83.195798949737437</v>
       </c>
       <c r="E1261" s="21">
@@ -53574,7 +53860,7 @@
         <v>16038.983021426331</v>
       </c>
       <c r="S1261" s="21">
-        <f t="shared" ref="S1261" si="7">M1261/E1261*10000</f>
+        <f t="shared" ref="S1261" si="21">M1261/E1261*10000</f>
         <v>144625.63590104898</v>
       </c>
       <c r="V1261" s="43">
@@ -53645,6 +53931,10 @@
       <c r="AC1262" s="21">
         <v>1.75</v>
       </c>
+      <c r="AE1262" s="21">
+        <f>(AC1262/2)^2*3.14159*E1262/10000</f>
+        <v>0.62224589557812493</v>
+      </c>
       <c r="AF1262" s="21">
         <v>2.12</v>
       </c>
@@ -53693,7 +53983,7 @@
         <v>1320.0378834186677</v>
       </c>
       <c r="S1263" s="21">
-        <f t="shared" ref="S1263:S1267" si="8">M1263/E1263*10000</f>
+        <f t="shared" ref="S1263:S1267" si="22">M1263/E1263*10000</f>
         <v>5102.5816908336592</v>
       </c>
       <c r="V1263" s="43">
@@ -53706,6 +53996,10 @@
       <c r="AC1263" s="21">
         <v>6.39</v>
       </c>
+      <c r="AE1263" s="21">
+        <f t="shared" ref="AE1263:AE1267" si="23">(AC1263/2)^2*3.14159*E1263/10000</f>
+        <v>8.2963613494973245</v>
+      </c>
       <c r="AF1263" s="21">
         <v>23.84</v>
       </c>
@@ -53754,7 +54048,7 @@
         <v>2668.5273415517941</v>
       </c>
       <c r="S1264" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>10315.14241032777</v>
       </c>
       <c r="V1264" s="43">
@@ -53767,6 +54061,10 @@
       <c r="AC1264" s="21">
         <v>8.25</v>
       </c>
+      <c r="AE1264" s="21">
+        <f t="shared" si="23"/>
+        <v>13.829097556828122</v>
+      </c>
       <c r="AF1264" s="21">
         <v>59.15</v>
       </c>
@@ -53815,7 +54113,7 @@
         <v>6693.037250926156</v>
       </c>
       <c r="S1265" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>26412.933113362888</v>
       </c>
       <c r="V1265" s="43">
@@ -53828,6 +54126,10 @@
       <c r="AC1265" s="21">
         <v>9.67</v>
       </c>
+      <c r="AE1265" s="21">
+        <f t="shared" si="23"/>
+        <v>18.610115703315849</v>
+      </c>
       <c r="AF1265" s="21">
         <v>105.61</v>
       </c>
@@ -53876,7 +54178,7 @@
         <v>8799.1791397126835</v>
       </c>
       <c r="S1266" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>35098.440924262795</v>
       </c>
       <c r="V1266" s="43">
@@ -53889,6 +54191,10 @@
       <c r="AC1266" s="21">
         <v>11.2</v>
       </c>
+      <c r="AE1266" s="21">
+        <f t="shared" si="23"/>
+        <v>24.699029783679997</v>
+      </c>
       <c r="AF1266" s="21">
         <v>158.74</v>
       </c>
@@ -53937,7 +54243,7 @@
         <v>12086.795940494598</v>
       </c>
       <c r="S1267" s="21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="22"/>
         <v>50361.649752060825</v>
       </c>
       <c r="V1267" s="43">
@@ -53950,6 +54256,10 @@
       <c r="AC1267" s="21">
         <v>12.4</v>
       </c>
+      <c r="AE1267" s="21">
+        <f t="shared" si="23"/>
+        <v>28.983052704000002</v>
+      </c>
       <c r="AF1267" s="21">
         <v>220.34</v>
       </c>
@@ -54019,7 +54329,7 @@
         <v>10</v>
       </c>
       <c r="D1271" s="21">
-        <f t="shared" ref="D1271:D1272" si="9">E1271/E$1226*100</f>
+        <f t="shared" ref="D1271:D1272" si="24">E1271/E$1226*100</f>
         <v>82.977127859017614</v>
       </c>
       <c r="E1271" s="21">
@@ -54047,7 +54357,7 @@
         <v>12.1</v>
       </c>
       <c r="D1272" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="24"/>
         <v>76.565429321334832</v>
       </c>
       <c r="E1272" s="21">
@@ -54072,7 +54382,7 @@
         <v>20675.87223779206</v>
       </c>
       <c r="S1272" s="21">
-        <f t="shared" ref="S1272" si="10">M1272/E1272*10000</f>
+        <f t="shared" ref="S1272" si="25">M1272/E1272*10000</f>
         <v>101253.04719780637</v>
       </c>
       <c r="V1272" s="43">
@@ -54160,6 +54470,10 @@
       <c r="AC1274" s="21">
         <v>3.6</v>
       </c>
+      <c r="AE1274" s="21">
+        <f>(AC1274/2)^2*3.14159*E1274/10000</f>
+        <v>2.2077712220399999</v>
+      </c>
       <c r="AN1274" s="21">
         <v>53</v>
       </c>
@@ -54210,6 +54524,10 @@
       <c r="AC1275" s="21">
         <v>7.16</v>
       </c>
+      <c r="AE1275" s="21">
+        <f t="shared" ref="AE1275:AE1277" si="26">(AC1275/2)^2*3.14159*E1275/10000</f>
+        <v>8.7332342870844002</v>
+      </c>
       <c r="AN1275" s="21">
         <v>92.1</v>
       </c>
@@ -54260,6 +54578,10 @@
       <c r="AC1276" s="21">
         <v>8.59</v>
       </c>
+      <c r="AE1276" s="21">
+        <f t="shared" si="26"/>
+        <v>12.570003372608774</v>
+      </c>
       <c r="AN1276" s="21">
         <v>125.3</v>
       </c>
@@ -54309,6 +54631,10 @@
       </c>
       <c r="AC1277" s="21">
         <v>10.74</v>
+      </c>
+      <c r="AE1277" s="21">
+        <f t="shared" si="26"/>
+        <v>19.6497771459399</v>
       </c>
       <c r="AN1277" s="21">
         <v>153.19999999999999</v>

</xml_diff>

<commit_message>
Added Wellstead site, and interception to nitens and globulus sites
</commit_message>
<xml_diff>
--- a/Tests/Validation/Eucalyptus/Observed.xlsx
+++ b/Tests/Validation/Eucalyptus/Observed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMxSourceTree\Tests\Validation\Eucalyptus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B76D46-1F85-408E-BD5C-74C550B98AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A4294A-144A-4BFC-A483-258A91EA32D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="653" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18223,10 +18223,10 @@
   <dimension ref="A1:BZ2742"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6330" ySplit="1575" topLeftCell="AA718" activePane="bottomRight"/>
+      <pane xSplit="6330" ySplit="1575" topLeftCell="A1504" activePane="bottomRight"/>
       <selection pane="topRight" activeCell="AC1" sqref="AC1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AF626" sqref="AF626:AF746"/>
+      <selection pane="bottomRight" activeCell="C1532" sqref="C1532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -55544,7 +55544,7 @@
         <v>0</v>
       </c>
       <c r="E1278" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1279" spans="1:40" s="21" customFormat="1">
@@ -55558,7 +55558,7 @@
         <v>0</v>
       </c>
       <c r="E1279" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1280" spans="1:40" s="21" customFormat="1">
@@ -55572,7 +55572,7 @@
         <v>0</v>
       </c>
       <c r="E1280" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1281" spans="1:34" s="21" customFormat="1">
@@ -55586,7 +55586,7 @@
         <v>0</v>
       </c>
       <c r="E1281" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1282" spans="1:34" s="21" customFormat="1">
@@ -55600,7 +55600,7 @@
         <v>0</v>
       </c>
       <c r="E1282" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1283" spans="1:34" s="21" customFormat="1">
@@ -55614,7 +55614,7 @@
         <v>0</v>
       </c>
       <c r="E1283" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1284" spans="1:34" s="21" customFormat="1">
@@ -55628,7 +55628,7 @@
         <v>0</v>
       </c>
       <c r="E1284" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1285" spans="1:34" s="21" customFormat="1">
@@ -55642,7 +55642,7 @@
         <v>0</v>
       </c>
       <c r="E1285" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1286" spans="1:34" s="21" customFormat="1">
@@ -55656,7 +55656,7 @@
         <v>0</v>
       </c>
       <c r="E1286" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1287" spans="1:34" s="21" customFormat="1">
@@ -55670,7 +55670,7 @@
         <v>0</v>
       </c>
       <c r="E1287" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1288" spans="1:34" s="21" customFormat="1">
@@ -55684,7 +55684,7 @@
         <v>0</v>
       </c>
       <c r="E1288" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1289" spans="1:34" s="21" customFormat="1">
@@ -58906,7 +58906,7 @@
         <v>0</v>
       </c>
       <c r="E1443" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1444" spans="1:34" s="21" customFormat="1">
@@ -58920,7 +58920,7 @@
         <v>0</v>
       </c>
       <c r="E1444" s="21">
-        <v>300</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1445" spans="1:34" s="21" customFormat="1">
@@ -58934,7 +58934,7 @@
         <v>0</v>
       </c>
       <c r="E1445" s="21">
-        <v>600</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1446" spans="1:34" s="21" customFormat="1">
@@ -58948,7 +58948,7 @@
         <v>0</v>
       </c>
       <c r="E1446" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1447" spans="1:34" s="21" customFormat="1">
@@ -58962,7 +58962,7 @@
         <v>0</v>
       </c>
       <c r="E1447" s="21">
-        <v>600</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1448" spans="1:34" s="21" customFormat="1">
@@ -58976,7 +58976,7 @@
         <v>0</v>
       </c>
       <c r="E1448" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1449" spans="1:34" s="21" customFormat="1">
@@ -58990,7 +58990,7 @@
         <v>0</v>
       </c>
       <c r="E1449" s="21">
-        <v>300</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1450" spans="1:34" s="21" customFormat="1">
@@ -59004,7 +59004,7 @@
         <v>0</v>
       </c>
       <c r="E1450" s="21">
-        <v>600</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1451" spans="1:34" s="21" customFormat="1">
@@ -59018,7 +59018,7 @@
         <v>0</v>
       </c>
       <c r="E1451" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1452" spans="1:34" s="21" customFormat="1">
@@ -59032,7 +59032,7 @@
         <v>0</v>
       </c>
       <c r="E1452" s="21">
-        <v>600</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1453" spans="1:34" s="21" customFormat="1">
@@ -59046,7 +59046,7 @@
         <v>0</v>
       </c>
       <c r="E1453" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1454" spans="1:34" s="21" customFormat="1">
@@ -63067,7 +63067,7 @@
         <v>0</v>
       </c>
       <c r="E1619" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1620" spans="1:34" s="21" customFormat="1">
@@ -63081,7 +63081,7 @@
         <v>0</v>
       </c>
       <c r="E1620" s="21">
-        <v>300</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1621" spans="1:34" s="21" customFormat="1">
@@ -63095,7 +63095,7 @@
         <v>0</v>
       </c>
       <c r="E1621" s="21">
-        <v>600</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1622" spans="1:34" s="21" customFormat="1">
@@ -63109,7 +63109,7 @@
         <v>0</v>
       </c>
       <c r="E1622" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1623" spans="1:34" s="21" customFormat="1">
@@ -63123,7 +63123,7 @@
         <v>0</v>
       </c>
       <c r="E1623" s="21">
-        <v>600</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1624" spans="1:34" s="21" customFormat="1">
@@ -63137,7 +63137,7 @@
         <v>0</v>
       </c>
       <c r="E1624" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1625" spans="1:34" s="21" customFormat="1">
@@ -63151,7 +63151,7 @@
         <v>0</v>
       </c>
       <c r="E1625" s="21">
-        <v>300</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1626" spans="1:34" s="21" customFormat="1">
@@ -63165,7 +63165,7 @@
         <v>0</v>
       </c>
       <c r="E1626" s="21">
-        <v>600</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1627" spans="1:34" s="21" customFormat="1">
@@ -63179,7 +63179,7 @@
         <v>0</v>
       </c>
       <c r="E1627" s="21">
-        <v>1200</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1628" spans="1:34" s="21" customFormat="1">
@@ -63193,7 +63193,7 @@
         <v>0</v>
       </c>
       <c r="E1628" s="21">
-        <v>600</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1629" spans="1:34" s="21" customFormat="1">

</xml_diff>